<commit_message>
Sofia | hydrostatick curve | fix
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/datasets/Stability/SSS_Sofia_Pantokarens_Angle_HydrostaticCurves.xlsx
+++ b/assets/fleet/9245263_sofia/datasets/Stability/SSS_Sofia_Pantokarens_Angle_HydrostaticCurves.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3EEB835-ADC4-4E27-B36A-6919876A269E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD9673A-310A-470A-93C1-B196742D1A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Angle" sheetId="1" r:id="rId1"/>
@@ -1307,8 +1307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A4FC80-BF2A-45A2-A621-AB74F1039367}">
   <dimension ref="A1:Y187"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1437,8 +1437,8 @@
       <c r="G2" s="6">
         <v>1669.5</v>
       </c>
-      <c r="H2" s="7">
-        <v>1.75</v>
+      <c r="H2" s="6">
+        <v>67.013000000000005</v>
       </c>
       <c r="I2" s="6">
         <v>30519.4</v>
@@ -1512,8 +1512,8 @@
       <c r="G3" s="6">
         <v>1675.1</v>
       </c>
-      <c r="H3" s="7">
-        <v>1.75</v>
+      <c r="H3" s="6">
+        <v>66.984999999999999</v>
       </c>
       <c r="I3" s="6">
         <v>30719</v>
@@ -1587,8 +1587,8 @@
       <c r="G4" s="6">
         <v>1680.7</v>
       </c>
-      <c r="H4" s="7">
-        <v>1.6500000000000057</v>
+      <c r="H4" s="6">
+        <v>66.945999999999998</v>
       </c>
       <c r="I4" s="6">
         <v>30916.3</v>
@@ -1662,8 +1662,8 @@
       <c r="G5" s="6">
         <v>1686.5</v>
       </c>
-      <c r="H5" s="7">
-        <v>1.6500000000000057</v>
+      <c r="H5" s="6">
+        <v>66.894999999999996</v>
       </c>
       <c r="I5" s="6">
         <v>31114.2</v>
@@ -1737,8 +1737,8 @@
       <c r="G6" s="6">
         <v>1692.2</v>
       </c>
-      <c r="H6" s="7">
-        <v>1.5499999999999972</v>
+      <c r="H6" s="6">
+        <v>66.826999999999998</v>
       </c>
       <c r="I6" s="6">
         <v>31312</v>
@@ -1812,8 +1812,8 @@
       <c r="G7" s="6">
         <v>1698.1</v>
       </c>
-      <c r="H7" s="7">
-        <v>1.4500000000000028</v>
+      <c r="H7" s="6">
+        <v>66.736000000000004</v>
       </c>
       <c r="I7" s="6">
         <v>31508.7</v>
@@ -1887,8 +1887,8 @@
       <c r="G8" s="6">
         <v>1703.7</v>
       </c>
-      <c r="H8" s="7">
-        <v>1.3499999999999943</v>
+      <c r="H8" s="6">
+        <v>66.613</v>
       </c>
       <c r="I8" s="6">
         <v>31706.5</v>
@@ -1962,8 +1962,8 @@
       <c r="G9" s="6">
         <v>1709.5</v>
       </c>
-      <c r="H9" s="7">
-        <v>1.25</v>
+      <c r="H9" s="6">
+        <v>66.471000000000004</v>
       </c>
       <c r="I9" s="6">
         <v>31907.4</v>
@@ -2037,8 +2037,8 @@
       <c r="G10" s="6">
         <v>1715.6</v>
       </c>
-      <c r="H10" s="7">
-        <v>1.0499999999999972</v>
+      <c r="H10" s="6">
+        <v>66.313999999999993</v>
       </c>
       <c r="I10" s="6">
         <v>32110.799999999999</v>
@@ -2112,8 +2112,8 @@
       <c r="G11" s="6">
         <v>1722</v>
       </c>
-      <c r="H11" s="7">
-        <v>0.84999999999999432</v>
+      <c r="H11" s="6">
+        <v>66.141000000000005</v>
       </c>
       <c r="I11" s="6">
         <v>32317.599999999999</v>
@@ -2187,8 +2187,8 @@
       <c r="G12" s="6">
         <v>1728.8</v>
       </c>
-      <c r="H12" s="7">
-        <v>0.75</v>
+      <c r="H12" s="6">
+        <v>65.954999999999998</v>
       </c>
       <c r="I12" s="6">
         <v>32530.400000000001</v>
@@ -2262,8 +2262,8 @@
       <c r="G13" s="6">
         <v>1736.5</v>
       </c>
-      <c r="H13" s="7">
-        <v>0.54999999999999716</v>
+      <c r="H13" s="6">
+        <v>65.753</v>
       </c>
       <c r="I13" s="6">
         <v>32750.3</v>
@@ -2337,8 +2337,8 @@
       <c r="G14" s="6">
         <v>1744.9</v>
       </c>
-      <c r="H14" s="7">
-        <v>0.25</v>
+      <c r="H14" s="6">
+        <v>65.534000000000006</v>
       </c>
       <c r="I14" s="6">
         <v>32978.199999999997</v>
@@ -2412,8 +2412,8 @@
       <c r="G15" s="6">
         <v>1754.3</v>
       </c>
-      <c r="H15" s="7">
-        <v>4.9999999999997158E-2</v>
+      <c r="H15" s="6">
+        <v>65.284999999999997</v>
       </c>
       <c r="I15" s="6">
         <v>33214.1</v>
@@ -2487,8 +2487,8 @@
       <c r="G16" s="6">
         <v>1764.4</v>
       </c>
-      <c r="H16" s="7">
-        <v>-0.25</v>
+      <c r="H16" s="6">
+        <v>65.004999999999995</v>
       </c>
       <c r="I16" s="6">
         <v>33461.9</v>
@@ -2562,8 +2562,8 @@
       <c r="G17" s="6">
         <v>1775.8</v>
       </c>
-      <c r="H17" s="7">
-        <v>-0.54999999999999716</v>
+      <c r="H17" s="6">
+        <v>64.695999999999998</v>
       </c>
       <c r="I17" s="6">
         <v>33724.6</v>
@@ -2637,8 +2637,8 @@
       <c r="G18" s="6">
         <v>1788.3</v>
       </c>
-      <c r="H18" s="7">
-        <v>-0.84999999999999432</v>
+      <c r="H18" s="6">
+        <v>64.37</v>
       </c>
       <c r="I18" s="6">
         <v>33999.1</v>
@@ -2712,8 +2712,8 @@
       <c r="G19" s="6">
         <v>1801.8</v>
       </c>
-      <c r="H19" s="7">
-        <v>-1.25</v>
+      <c r="H19" s="6">
+        <v>64.034000000000006</v>
       </c>
       <c r="I19" s="6">
         <v>34288.1</v>
@@ -2787,8 +2787,8 @@
       <c r="G20" s="6">
         <v>1815.7</v>
       </c>
-      <c r="H20" s="7">
-        <v>-1.5499999999999972</v>
+      <c r="H20" s="6">
+        <v>63.723999999999997</v>
       </c>
       <c r="I20" s="6">
         <v>34592.9</v>
@@ -2862,8 +2862,8 @@
       <c r="G21" s="6">
         <v>1831</v>
       </c>
-      <c r="H21" s="7">
-        <v>-1.8500000000000014</v>
+      <c r="H21" s="6">
+        <v>63.41</v>
       </c>
       <c r="I21" s="6">
         <v>34906.9</v>
@@ -2937,8 +2937,8 @@
       <c r="G22" s="6">
         <v>1846.6</v>
       </c>
-      <c r="H22" s="7">
-        <v>-2.1499999999999986</v>
+      <c r="H22" s="6">
+        <v>63.109000000000002</v>
       </c>
       <c r="I22" s="6">
         <v>35230.400000000001</v>
@@ -3012,8 +3012,8 @@
       <c r="G23" s="6">
         <v>1861.9</v>
       </c>
-      <c r="H23" s="7">
-        <v>-2.4500000000000028</v>
+      <c r="H23" s="6">
+        <v>62.831000000000003</v>
       </c>
       <c r="I23" s="6">
         <v>35561.9</v>
@@ -3087,8 +3087,8 @@
       <c r="G24" s="6">
         <v>1876.2</v>
       </c>
-      <c r="H24" s="7">
-        <v>-2.6499999999999986</v>
+      <c r="H24" s="6">
+        <v>62.63</v>
       </c>
       <c r="I24" s="6">
         <v>35899.199999999997</v>
@@ -3162,8 +3162,8 @@
       <c r="G25" s="6">
         <v>1889.5</v>
       </c>
-      <c r="H25" s="7">
-        <v>-2.75</v>
+      <c r="H25" s="6">
+        <v>62.487000000000002</v>
       </c>
       <c r="I25" s="6">
         <v>36238.300000000003</v>
@@ -3237,8 +3237,8 @@
       <c r="G26" s="6">
         <v>1902.1</v>
       </c>
-      <c r="H26" s="7">
-        <v>-2.8500000000000014</v>
+      <c r="H26" s="6">
+        <v>62.389000000000003</v>
       </c>
       <c r="I26" s="6">
         <v>36577.300000000003</v>
@@ -3312,8 +3312,8 @@
       <c r="G27" s="6">
         <v>1913.9</v>
       </c>
-      <c r="H27" s="7">
-        <v>-2.9500000000000028</v>
+      <c r="H27" s="6">
+        <v>62.326999999999998</v>
       </c>
       <c r="I27" s="6">
         <v>36920.699999999997</v>
@@ -3387,8 +3387,8 @@
       <c r="G28" s="6">
         <v>1925.7</v>
       </c>
-      <c r="H28" s="7">
-        <v>-2.9500000000000028</v>
+      <c r="H28" s="6">
+        <v>62.293999999999997</v>
       </c>
       <c r="I28" s="6">
         <v>37255.4</v>
@@ -3462,8 +3462,8 @@
       <c r="G29" s="6">
         <v>1936.8</v>
       </c>
-      <c r="H29" s="7">
-        <v>-2.9500000000000028</v>
+      <c r="H29" s="6">
+        <v>62.287999999999997</v>
       </c>
       <c r="I29" s="6">
         <v>37591.199999999997</v>
@@ -3537,8 +3537,8 @@
       <c r="G30" s="6">
         <v>1947.7</v>
       </c>
-      <c r="H30" s="7">
-        <v>-2.9500000000000028</v>
+      <c r="H30" s="6">
+        <v>62.296999999999997</v>
       </c>
       <c r="I30" s="6">
         <v>37924.300000000003</v>
@@ -3612,8 +3612,8 @@
       <c r="G31" s="6">
         <v>1958.6</v>
       </c>
-      <c r="H31" s="7">
-        <v>-2.9500000000000028</v>
+      <c r="H31" s="6">
+        <v>62.33</v>
       </c>
       <c r="I31" s="6">
         <v>38246</v>
@@ -3687,8 +3687,8 @@
       <c r="G32" s="6">
         <v>1969.2</v>
       </c>
-      <c r="H32" s="7">
-        <v>-2.8500000000000014</v>
+      <c r="H32" s="6">
+        <v>62.38</v>
       </c>
       <c r="I32" s="6">
         <v>38566.699999999997</v>
@@ -3762,8 +3762,8 @@
       <c r="G33" s="6">
         <v>1669.6</v>
       </c>
-      <c r="H33" s="7">
-        <v>1.75</v>
+      <c r="H33" s="6">
+        <v>66.959000000000003</v>
       </c>
       <c r="I33" s="6">
         <v>30534.2</v>
@@ -3837,8 +3837,8 @@
       <c r="G34" s="6">
         <v>1675.4</v>
       </c>
-      <c r="H34" s="7">
-        <v>1.6500000000000057</v>
+      <c r="H34" s="6">
+        <v>66.933000000000007</v>
       </c>
       <c r="I34" s="6">
         <v>30737</v>
@@ -3912,8 +3912,8 @@
       <c r="G35" s="6">
         <v>1681.2</v>
       </c>
-      <c r="H35" s="7">
-        <v>1.6500000000000057</v>
+      <c r="H35" s="6">
+        <v>66.893000000000001</v>
       </c>
       <c r="I35" s="6">
         <v>30937</v>
@@ -3987,8 +3987,8 @@
       <c r="G36" s="6">
         <v>1687.1</v>
       </c>
-      <c r="H36" s="7">
-        <v>1.5499999999999972</v>
+      <c r="H36" s="6">
+        <v>66.84</v>
       </c>
       <c r="I36" s="6">
         <v>31137.599999999999</v>
@@ -4062,8 +4062,8 @@
       <c r="G37" s="6">
         <v>1693.1</v>
       </c>
-      <c r="H37" s="7">
-        <v>1.5499999999999972</v>
+      <c r="H37" s="6">
+        <v>66.77</v>
       </c>
       <c r="I37" s="6">
         <v>31337.5</v>
@@ -4137,8 +4137,8 @@
       <c r="G38" s="6">
         <v>1699.1</v>
       </c>
-      <c r="H38" s="7">
-        <v>1.4500000000000028</v>
+      <c r="H38" s="6">
+        <v>66.680000000000007</v>
       </c>
       <c r="I38" s="6">
         <v>31536.3</v>
@@ -4212,8 +4212,8 @@
       <c r="G39" s="6">
         <v>1705.2</v>
       </c>
-      <c r="H39" s="7">
-        <v>1.3499999999999943</v>
+      <c r="H39" s="6">
+        <v>66.561000000000007</v>
       </c>
       <c r="I39" s="6">
         <v>31736.3</v>
@@ -4287,8 +4287,8 @@
       <c r="G40" s="6">
         <v>1711.1</v>
       </c>
-      <c r="H40" s="7">
-        <v>1.1500000000000057</v>
+      <c r="H40" s="6">
+        <v>66.415999999999997</v>
       </c>
       <c r="I40" s="6">
         <v>31939.1</v>
@@ -4362,8 +4362,8 @@
       <c r="G41" s="6">
         <v>1717.4</v>
       </c>
-      <c r="H41" s="7">
-        <v>1.0499999999999972</v>
+      <c r="H41" s="6">
+        <v>66.254999999999995</v>
       </c>
       <c r="I41" s="6">
         <v>32144.3</v>
@@ -4437,8 +4437,8 @@
       <c r="G42" s="6">
         <v>1723.9</v>
       </c>
-      <c r="H42" s="7">
-        <v>0.84999999999999432</v>
+      <c r="H42" s="6">
+        <v>66.078000000000003</v>
       </c>
       <c r="I42" s="6">
         <v>32352.9</v>
@@ -4512,8 +4512,8 @@
       <c r="G43" s="6">
         <v>1731</v>
       </c>
-      <c r="H43" s="7">
-        <v>0.65000000000000568</v>
+      <c r="H43" s="6">
+        <v>65.882999999999996</v>
       </c>
       <c r="I43" s="6">
         <v>32567.5</v>
@@ -4587,8 +4587,8 @@
       <c r="G44" s="6">
         <v>1738.8</v>
       </c>
-      <c r="H44" s="7">
-        <v>0.45000000000000284</v>
+      <c r="H44" s="6">
+        <v>65.67</v>
       </c>
       <c r="I44" s="6">
         <v>32790.199999999997</v>
@@ -4662,8 +4662,8 @@
       <c r="G45" s="6">
         <v>1747.6</v>
       </c>
-      <c r="H45" s="7">
-        <v>0.15000000000000568</v>
+      <c r="H45" s="6">
+        <v>65.438999999999993</v>
       </c>
       <c r="I45" s="6">
         <v>33019.699999999997</v>
@@ -4737,8 +4737,8 @@
       <c r="G46" s="6">
         <v>1757.3</v>
       </c>
-      <c r="H46" s="7">
-        <v>-4.9999999999997158E-2</v>
+      <c r="H46" s="6">
+        <v>65.177999999999997</v>
       </c>
       <c r="I46" s="6">
         <v>33257.699999999997</v>
@@ -4812,8 +4812,8 @@
       <c r="G47" s="6">
         <v>1767.9</v>
       </c>
-      <c r="H47" s="7">
-        <v>-0.34999999999999432</v>
+      <c r="H47" s="6">
+        <v>64.885999999999996</v>
       </c>
       <c r="I47" s="6">
         <v>33509.800000000003</v>
@@ -4887,8 +4887,8 @@
       <c r="G48" s="6">
         <v>1779.6</v>
       </c>
-      <c r="H48" s="7">
-        <v>-0.65000000000000568</v>
+      <c r="H48" s="6">
+        <v>64.56</v>
       </c>
       <c r="I48" s="6">
         <v>33775.300000000003</v>
@@ -4962,8 +4962,8 @@
       <c r="G49" s="6">
         <v>1792.4</v>
       </c>
-      <c r="H49" s="7">
-        <v>-1.0499999999999972</v>
+      <c r="H49" s="6">
+        <v>64.216999999999999</v>
       </c>
       <c r="I49" s="6">
         <v>34052.5</v>
@@ -5037,8 +5037,8 @@
       <c r="G50" s="6">
         <v>1805.6</v>
       </c>
-      <c r="H50" s="7">
-        <v>-1.3500000000000014</v>
+      <c r="H50" s="6">
+        <v>63.875999999999998</v>
       </c>
       <c r="I50" s="6">
         <v>34345.4</v>
@@ -5112,8 +5112,8 @@
       <c r="G51" s="6">
         <v>1819.7</v>
       </c>
-      <c r="H51" s="7">
-        <v>-1.75</v>
+      <c r="H51" s="6">
+        <v>63.545999999999999</v>
       </c>
       <c r="I51" s="6">
         <v>34652</v>
@@ -5187,8 +5187,8 @@
       <c r="G52" s="6">
         <v>1834.8</v>
       </c>
-      <c r="H52" s="7">
-        <v>-2.0499999999999972</v>
+      <c r="H52" s="6">
+        <v>63.223999999999997</v>
       </c>
       <c r="I52" s="6">
         <v>34966.1</v>
@@ -5262,8 +5262,8 @@
       <c r="G53" s="6">
         <v>1850.4</v>
       </c>
-      <c r="H53" s="7">
-        <v>-2.3500000000000014</v>
+      <c r="H53" s="6">
+        <v>62.914999999999999</v>
       </c>
       <c r="I53" s="6">
         <v>35291</v>
@@ -5337,8 +5337,8 @@
       <c r="G54" s="6">
         <v>1864.9</v>
       </c>
-      <c r="H54" s="7">
-        <v>-2.5499999999999972</v>
+      <c r="H54" s="6">
+        <v>62.658999999999999</v>
       </c>
       <c r="I54" s="6">
         <v>35620.199999999997</v>
@@ -5412,8 +5412,8 @@
       <c r="G55" s="6">
         <v>1878.4</v>
       </c>
-      <c r="H55" s="7">
-        <v>-2.75</v>
+      <c r="H55" s="6">
+        <v>62.469000000000001</v>
       </c>
       <c r="I55" s="6">
         <v>35956.1</v>
@@ -5487,8 +5487,8 @@
       <c r="G56" s="6">
         <v>1891.2</v>
       </c>
-      <c r="H56" s="7">
-        <v>-2.9500000000000028</v>
+      <c r="H56" s="6">
+        <v>62.334000000000003</v>
       </c>
       <c r="I56" s="6">
         <v>36290.300000000003</v>
@@ -5562,8 +5562,8 @@
       <c r="G57" s="6">
         <v>1903.2</v>
       </c>
-      <c r="H57" s="7">
-        <v>-2.9500000000000028</v>
+      <c r="H57" s="6">
+        <v>62.250999999999998</v>
       </c>
       <c r="I57" s="6">
         <v>36626.400000000001</v>
@@ -5637,8 +5637,8 @@
       <c r="G58" s="6">
         <v>1914.7</v>
       </c>
-      <c r="H58" s="7">
-        <v>-3.0499999999999972</v>
+      <c r="H58" s="6">
+        <v>62.192</v>
       </c>
       <c r="I58" s="6">
         <v>36964.9</v>
@@ -5712,8 +5712,8 @@
       <c r="G59" s="6">
         <v>1926</v>
       </c>
-      <c r="H59" s="7">
-        <v>-3.0499999999999972</v>
+      <c r="H59" s="6">
+        <v>62.164000000000001</v>
       </c>
       <c r="I59" s="6">
         <v>37293.1</v>
@@ -5787,8 +5787,8 @@
       <c r="G60" s="6">
         <v>1937</v>
       </c>
-      <c r="H60" s="7">
-        <v>-3.0499999999999972</v>
+      <c r="H60" s="6">
+        <v>62.161999999999999</v>
       </c>
       <c r="I60" s="6">
         <v>37626.400000000001</v>
@@ -5862,8 +5862,8 @@
       <c r="G61" s="6">
         <v>1947.8</v>
       </c>
-      <c r="H61" s="7">
-        <v>-3.0499999999999972</v>
+      <c r="H61" s="6">
+        <v>62.171999999999997</v>
       </c>
       <c r="I61" s="6">
         <v>37950.699999999997</v>
@@ -5937,8 +5937,8 @@
       <c r="G62" s="6">
         <v>1958.3</v>
       </c>
-      <c r="H62" s="7">
-        <v>-3.0499999999999972</v>
+      <c r="H62" s="6">
+        <v>62.207000000000001</v>
       </c>
       <c r="I62" s="6">
         <v>38267.699999999997</v>
@@ -6012,8 +6012,8 @@
       <c r="G63" s="6">
         <v>1968.7</v>
       </c>
-      <c r="H63" s="7">
-        <v>-2.9500000000000028</v>
+      <c r="H63" s="6">
+        <v>62.26</v>
       </c>
       <c r="I63" s="6">
         <v>38585.300000000003</v>
@@ -6087,8 +6087,8 @@
       <c r="G64" s="6">
         <v>1669.6</v>
       </c>
-      <c r="H64" s="7">
-        <v>1.6500000000000057</v>
+      <c r="H64" s="6">
+        <v>66.878</v>
       </c>
       <c r="I64" s="6">
         <v>30554.2</v>
@@ -6162,8 +6162,8 @@
       <c r="G65" s="6">
         <v>1675.9</v>
       </c>
-      <c r="H65" s="7">
-        <v>1.6500000000000057</v>
+      <c r="H65" s="6">
+        <v>66.86</v>
       </c>
       <c r="I65" s="6">
         <v>30761.7</v>
@@ -6237,8 +6237,8 @@
       <c r="G66" s="6">
         <v>1681.8</v>
       </c>
-      <c r="H66" s="7">
-        <v>1.5499999999999972</v>
+      <c r="H66" s="6">
+        <v>66.816999999999993</v>
       </c>
       <c r="I66" s="6">
         <v>30966.2</v>
@@ -6312,8 +6312,8 @@
       <c r="G67" s="6">
         <v>1687.9</v>
       </c>
-      <c r="H67" s="7">
-        <v>1.5499999999999972</v>
+      <c r="H67" s="6">
+        <v>66.759</v>
       </c>
       <c r="I67" s="6">
         <v>31170.3</v>
@@ -6387,8 +6387,8 @@
       <c r="G68" s="6">
         <v>1694.2</v>
       </c>
-      <c r="H68" s="7">
-        <v>1.4500000000000028</v>
+      <c r="H68" s="6">
+        <v>66.686000000000007</v>
       </c>
       <c r="I68" s="6">
         <v>31373.3</v>
@@ -6462,8 +6462,8 @@
       <c r="G69" s="6">
         <v>1700.6</v>
       </c>
-      <c r="H69" s="7">
-        <v>1.3499999999999943</v>
+      <c r="H69" s="6">
+        <v>66.594999999999999</v>
       </c>
       <c r="I69" s="6">
         <v>31575.3</v>
@@ -6537,8 +6537,8 @@
       <c r="G70" s="6">
         <v>1707.1</v>
       </c>
-      <c r="H70" s="7">
-        <v>1.25</v>
+      <c r="H70" s="6">
+        <v>66.480999999999995</v>
       </c>
       <c r="I70" s="6">
         <v>31778.3</v>
@@ -6612,8 +6612,8 @@
       <c r="G71" s="6">
         <v>1713.4</v>
       </c>
-      <c r="H71" s="7">
-        <v>1.0499999999999972</v>
+      <c r="H71" s="6">
+        <v>66.335999999999999</v>
       </c>
       <c r="I71" s="6">
         <v>31983.4</v>
@@ -6687,8 +6687,8 @@
       <c r="G72" s="6">
         <v>1719.9</v>
       </c>
-      <c r="H72" s="7">
-        <v>0.95000000000000284</v>
+      <c r="H72" s="6">
+        <v>66.168999999999997</v>
       </c>
       <c r="I72" s="6">
         <v>32191.7</v>
@@ -6762,8 +6762,8 @@
       <c r="G73" s="6">
         <v>1726.8</v>
       </c>
-      <c r="H73" s="7">
-        <v>0.75</v>
+      <c r="H73" s="6">
+        <v>65.986999999999995</v>
       </c>
       <c r="I73" s="6">
         <v>32403.3</v>
@@ -6837,8 +6837,8 @@
       <c r="G74" s="6">
         <v>1734.2</v>
       </c>
-      <c r="H74" s="7">
-        <v>0.54999999999999716</v>
+      <c r="H74" s="6">
+        <v>65.778999999999996</v>
       </c>
       <c r="I74" s="6">
         <v>32620.6</v>
@@ -6912,8 +6912,8 @@
       <c r="G75" s="6">
         <v>1742.4</v>
       </c>
-      <c r="H75" s="7">
-        <v>0.34999999999999432</v>
+      <c r="H75" s="6">
+        <v>65.552000000000007</v>
       </c>
       <c r="I75" s="6">
         <v>32846.9</v>
@@ -6987,8 +6987,8 @@
       <c r="G76" s="6">
         <v>1751.6</v>
       </c>
-      <c r="H76" s="7">
-        <v>4.9999999999997158E-2</v>
+      <c r="H76" s="6">
+        <v>65.299000000000007</v>
       </c>
       <c r="I76" s="6">
         <v>33079.5</v>
@@ -7062,8 +7062,8 @@
       <c r="G77" s="6">
         <v>1761.8</v>
       </c>
-      <c r="H77" s="7">
-        <v>-0.25</v>
+      <c r="H77" s="6">
+        <v>65.022000000000006</v>
       </c>
       <c r="I77" s="6">
         <v>33321.4</v>
@@ -7137,8 +7137,8 @@
       <c r="G78" s="6">
         <v>1773.1</v>
       </c>
-      <c r="H78" s="7">
-        <v>-0.54999999999999716</v>
+      <c r="H78" s="6">
+        <v>64.710999999999999</v>
       </c>
       <c r="I78" s="6">
         <v>33579.5</v>
@@ -7212,8 +7212,8 @@
       <c r="G79" s="6">
         <v>1785.2</v>
       </c>
-      <c r="H79" s="7">
-        <v>-0.84999999999999432</v>
+      <c r="H79" s="6">
+        <v>64.367000000000004</v>
       </c>
       <c r="I79" s="6">
         <v>33848.699999999997</v>
@@ -7287,8 +7287,8 @@
       <c r="G80" s="6">
         <v>1798.1</v>
       </c>
-      <c r="H80" s="7">
-        <v>-1.25</v>
+      <c r="H80" s="6">
+        <v>64.007000000000005</v>
       </c>
       <c r="I80" s="6">
         <v>34130.199999999997</v>
@@ -7362,8 +7362,8 @@
       <c r="G81" s="6">
         <v>1811.2</v>
       </c>
-      <c r="H81" s="7">
-        <v>-1.5499999999999972</v>
+      <c r="H81" s="6">
+        <v>63.661999999999999</v>
       </c>
       <c r="I81" s="6">
         <v>34428.800000000003</v>
@@ -7437,8 +7437,8 @@
       <c r="G82" s="6">
         <v>1825.5</v>
       </c>
-      <c r="H82" s="7">
-        <v>-1.9500000000000028</v>
+      <c r="H82" s="6">
+        <v>63.302999999999997</v>
       </c>
       <c r="I82" s="6">
         <v>34736.199999999997</v>
@@ -7512,8 +7512,8 @@
       <c r="G83" s="6">
         <v>1840.4</v>
       </c>
-      <c r="H83" s="7">
-        <v>-2.25</v>
+      <c r="H83" s="6">
+        <v>62.966000000000001</v>
       </c>
       <c r="I83" s="6">
         <v>35051.300000000003</v>
@@ -7587,8 +7587,8 @@
       <c r="G84" s="6">
         <v>1855.2</v>
       </c>
-      <c r="H84" s="7">
-        <v>-2.5499999999999972</v>
+      <c r="H84" s="6">
+        <v>62.665999999999997</v>
       </c>
       <c r="I84" s="6">
         <v>35375.9</v>
@@ -7662,8 +7662,8 @@
       <c r="G85" s="6">
         <v>1868.8</v>
       </c>
-      <c r="H85" s="7">
-        <v>-2.8500000000000014</v>
+      <c r="H85" s="6">
+        <v>62.436999999999998</v>
       </c>
       <c r="I85" s="6">
         <v>35703.300000000003</v>
@@ -7737,8 +7737,8 @@
       <c r="G86" s="6">
         <v>1881.3</v>
       </c>
-      <c r="H86" s="7">
-        <v>-2.9500000000000028</v>
+      <c r="H86" s="6">
+        <v>62.262</v>
       </c>
       <c r="I86" s="6">
         <v>36035.1</v>
@@ -7812,8 +7812,8 @@
       <c r="G87" s="6">
         <v>1893.2</v>
       </c>
-      <c r="H87" s="7">
-        <v>-3.1499999999999986</v>
+      <c r="H87" s="6">
+        <v>62.140999999999998</v>
       </c>
       <c r="I87" s="6">
         <v>36363.599999999999</v>
@@ -7887,8 +7887,8 @@
       <c r="G88" s="6">
         <v>1904.6</v>
       </c>
-      <c r="H88" s="7">
-        <v>-3.1499999999999986</v>
+      <c r="H88" s="6">
+        <v>62.064999999999998</v>
       </c>
       <c r="I88" s="6">
         <v>36696.800000000003</v>
@@ -7962,8 +7962,8 @@
       <c r="G89" s="6">
         <v>1915.8</v>
       </c>
-      <c r="H89" s="7">
-        <v>-3.25</v>
+      <c r="H89" s="6">
+        <v>62.011000000000003</v>
       </c>
       <c r="I89" s="6">
         <v>37023.4</v>
@@ -8037,8 +8037,8 @@
       <c r="G90" s="6">
         <v>1926.5</v>
       </c>
-      <c r="H90" s="7">
-        <v>-3.25</v>
+      <c r="H90" s="6">
+        <v>61.988</v>
       </c>
       <c r="I90" s="6">
         <v>37347.599999999999</v>
@@ -8112,8 +8112,8 @@
       <c r="G91" s="6">
         <v>1937.2</v>
       </c>
-      <c r="H91" s="7">
-        <v>-3.25</v>
+      <c r="H91" s="6">
+        <v>61.99</v>
       </c>
       <c r="I91" s="6">
         <v>37674.1</v>
@@ -8187,8 +8187,8 @@
       <c r="G92" s="6">
         <v>1947.6</v>
       </c>
-      <c r="H92" s="7">
-        <v>-3.25</v>
+      <c r="H92" s="6">
+        <v>62.006999999999998</v>
       </c>
       <c r="I92" s="6">
         <v>37986.199999999997</v>
@@ -8262,8 +8262,8 @@
       <c r="G93" s="6">
         <v>1957.7</v>
       </c>
-      <c r="H93" s="7">
-        <v>-3.25</v>
+      <c r="H93" s="6">
+        <v>62.042999999999999</v>
       </c>
       <c r="I93" s="6">
         <v>38298.199999999997</v>
@@ -8337,8 +8337,8 @@
       <c r="G94" s="6">
         <v>1968</v>
       </c>
-      <c r="H94" s="7">
-        <v>-3.1499999999999986</v>
+      <c r="H94" s="6">
+        <v>62.095999999999997</v>
       </c>
       <c r="I94" s="6">
         <v>38607.4</v>
@@ -8412,8 +8412,8 @@
       <c r="G95" s="6">
         <v>1666.8</v>
       </c>
-      <c r="H95" s="7">
-        <v>1.3499999999999943</v>
+      <c r="H95" s="6">
+        <v>66.631</v>
       </c>
       <c r="I95" s="6">
         <v>30588.1</v>
@@ -8487,8 +8487,8 @@
       <c r="G96" s="6">
         <v>1676.5</v>
       </c>
-      <c r="H96" s="7">
-        <v>1.4500000000000028</v>
+      <c r="H96" s="6">
+        <v>66.715000000000003</v>
       </c>
       <c r="I96" s="6">
         <v>30803.5</v>
@@ -8562,8 +8562,8 @@
       <c r="G97" s="6">
         <v>1683.1</v>
       </c>
-      <c r="H97" s="7">
-        <v>1.4500000000000028</v>
+      <c r="H97" s="6">
+        <v>66.676000000000002</v>
       </c>
       <c r="I97" s="6">
         <v>31016.799999999999</v>
@@ -8637,8 +8637,8 @@
       <c r="G98" s="6">
         <v>1689.6</v>
       </c>
-      <c r="H98" s="7">
-        <v>1.3499999999999943</v>
+      <c r="H98" s="6">
+        <v>66.611000000000004</v>
       </c>
       <c r="I98" s="6">
         <v>31226.9</v>
@@ -8712,8 +8712,8 @@
       <c r="G99" s="6">
         <v>1696.3</v>
       </c>
-      <c r="H99" s="7">
-        <v>1.25</v>
+      <c r="H99" s="6">
+        <v>66.53</v>
       </c>
       <c r="I99" s="6">
         <v>31435.5</v>
@@ -8787,8 +8787,8 @@
       <c r="G100" s="6">
         <v>1703.2</v>
       </c>
-      <c r="H100" s="7">
-        <v>1.1500000000000057</v>
+      <c r="H100" s="6">
+        <v>66.433000000000007</v>
       </c>
       <c r="I100" s="6">
         <v>31644</v>
@@ -8862,8 +8862,8 @@
       <c r="G101" s="6">
         <v>1710.3</v>
       </c>
-      <c r="H101" s="7">
-        <v>1.0499999999999972</v>
+      <c r="H101" s="6">
+        <v>66.319000000000003</v>
       </c>
       <c r="I101" s="6">
         <v>31853.1</v>
@@ -8937,8 +8937,8 @@
       <c r="G102" s="6">
         <v>1717.5</v>
       </c>
-      <c r="H102" s="7">
-        <v>0.95000000000000284</v>
+      <c r="H102" s="6">
+        <v>66.180000000000007</v>
       </c>
       <c r="I102" s="6">
         <v>32063.4</v>
@@ -9012,8 +9012,8 @@
       <c r="G103" s="6">
         <v>1724.6</v>
       </c>
-      <c r="H103" s="7">
-        <v>0.75</v>
+      <c r="H103" s="6">
+        <v>66.009</v>
       </c>
       <c r="I103" s="6">
         <v>32276.799999999999</v>
@@ -9087,8 +9087,8 @@
       <c r="G104" s="6">
         <v>1732.1</v>
       </c>
-      <c r="H104" s="7">
-        <v>0.54999999999999716</v>
+      <c r="H104" s="6">
+        <v>65.808999999999997</v>
       </c>
       <c r="I104" s="6">
         <v>32494.6</v>
@@ -9162,8 +9162,8 @@
       <c r="G105" s="6">
         <v>1740.3</v>
       </c>
-      <c r="H105" s="7">
-        <v>0.34999999999999432</v>
+      <c r="H105" s="6">
+        <v>65.584999999999994</v>
       </c>
       <c r="I105" s="6">
         <v>32719</v>
@@ -9237,8 +9237,8 @@
       <c r="G106" s="6">
         <v>1749.3</v>
       </c>
-      <c r="H106" s="7">
-        <v>4.9999999999997158E-2</v>
+      <c r="H106" s="6">
+        <v>65.326999999999998</v>
       </c>
       <c r="I106" s="6">
         <v>32950.199999999997</v>
@@ -9312,8 +9312,8 @@
       <c r="G107" s="6">
         <v>1759.2</v>
       </c>
-      <c r="H107" s="7">
-        <v>-0.25</v>
+      <c r="H107" s="6">
+        <v>65.039000000000001</v>
       </c>
       <c r="I107" s="6">
         <v>33189.5</v>
@@ -9387,8 +9387,8 @@
       <c r="G108" s="6">
         <v>1770.3</v>
       </c>
-      <c r="H108" s="7">
-        <v>-0.54999999999999716</v>
+      <c r="H108" s="6">
+        <v>64.722999999999999</v>
       </c>
       <c r="I108" s="6">
         <v>33442.199999999997</v>
@@ -9462,8 +9462,8 @@
       <c r="G109" s="6">
         <v>1782.5</v>
       </c>
-      <c r="H109" s="7">
-        <v>-0.84999999999999432</v>
+      <c r="H109" s="6">
+        <v>64.379000000000005</v>
       </c>
       <c r="I109" s="6">
         <v>33707.9</v>
@@ -9537,8 +9537,8 @@
       <c r="G110" s="6">
         <v>1795.5</v>
       </c>
-      <c r="H110" s="7">
-        <v>-1.25</v>
+      <c r="H110" s="6">
+        <v>64.013999999999996</v>
       </c>
       <c r="I110" s="6">
         <v>33985</v>
@@ -9612,8 +9612,8 @@
       <c r="G111" s="6">
         <v>1808.3</v>
       </c>
-      <c r="H111" s="7">
-        <v>-1.5499999999999972</v>
+      <c r="H111" s="6">
+        <v>63.651000000000003</v>
       </c>
       <c r="I111" s="6">
         <v>34276.199999999997</v>
@@ -9687,8 +9687,8 @@
       <c r="G112" s="6">
         <v>1822</v>
       </c>
-      <c r="H112" s="7">
-        <v>-1.9500000000000028</v>
+      <c r="H112" s="6">
+        <v>63.267000000000003</v>
       </c>
       <c r="I112" s="6">
         <v>34579.199999999997</v>
@@ -9762,8 +9762,8 @@
       <c r="G113" s="6">
         <v>1836.1</v>
       </c>
-      <c r="H113" s="7">
-        <v>-2.3500000000000014</v>
+      <c r="H113" s="6">
+        <v>62.892000000000003</v>
       </c>
       <c r="I113" s="6">
         <v>34888.6</v>
@@ -9837,8 +9837,8 @@
       <c r="G114" s="6">
         <v>1850</v>
       </c>
-      <c r="H114" s="7">
-        <v>-2.75</v>
+      <c r="H114" s="6">
+        <v>62.548999999999999</v>
       </c>
       <c r="I114" s="6">
         <v>35205.4</v>
@@ -9912,8 +9912,8 @@
       <c r="G115" s="6">
         <v>1862.7</v>
       </c>
-      <c r="H115" s="7">
-        <v>-2.9500000000000028</v>
+      <c r="H115" s="6">
+        <v>62.289000000000001</v>
       </c>
       <c r="I115" s="6">
         <v>35525.9</v>
@@ -9987,8 +9987,8 @@
       <c r="G116" s="6">
         <v>1874.7</v>
       </c>
-      <c r="H116" s="7">
-        <v>-3.1499999999999986</v>
+      <c r="H116" s="6">
+        <v>62.093000000000004</v>
       </c>
       <c r="I116" s="6">
         <v>35850.6</v>
@@ -10062,8 +10062,8 @@
       <c r="G117" s="6">
         <v>1885.9</v>
       </c>
-      <c r="H117" s="7">
-        <v>-3.3500000000000014</v>
+      <c r="H117" s="6">
+        <v>61.945</v>
       </c>
       <c r="I117" s="6">
         <v>36169.4</v>
@@ -10137,8 +10137,8 @@
       <c r="G118" s="6">
         <v>1896.4</v>
       </c>
-      <c r="H118" s="7">
-        <v>-3.4500000000000028</v>
+      <c r="H118" s="6">
+        <v>61.835999999999999</v>
       </c>
       <c r="I118" s="6">
         <v>36493.9</v>
@@ -10212,8 +10212,8 @@
       <c r="G119" s="6">
         <v>1907</v>
       </c>
-      <c r="H119" s="7">
-        <v>-3.4500000000000028</v>
+      <c r="H119" s="6">
+        <v>61.76</v>
       </c>
       <c r="I119" s="6">
         <v>36812.699999999997</v>
@@ -10287,8 +10287,8 @@
       <c r="G120" s="6">
         <v>1917.3</v>
       </c>
-      <c r="H120" s="7">
-        <v>-3.5499999999999972</v>
+      <c r="H120" s="6">
+        <v>61.722000000000001</v>
       </c>
       <c r="I120" s="6">
         <v>37125.300000000003</v>
@@ -10362,8 +10362,8 @@
       <c r="G121" s="6">
         <v>1927.4</v>
       </c>
-      <c r="H121" s="7">
-        <v>-3.5499999999999972</v>
+      <c r="H121" s="6">
+        <v>61.704000000000001</v>
       </c>
       <c r="I121" s="6">
         <v>37443.4</v>
@@ -10437,8 +10437,8 @@
       <c r="G122" s="6">
         <v>1937.3</v>
       </c>
-      <c r="H122" s="7">
-        <v>-3.5499999999999972</v>
+      <c r="H122" s="6">
+        <v>61.704000000000001</v>
       </c>
       <c r="I122" s="6">
         <v>37746.199999999997</v>
@@ -10512,8 +10512,8 @@
       <c r="G123" s="6">
         <v>1947.2</v>
       </c>
-      <c r="H123" s="7">
-        <v>-3.5499999999999972</v>
+      <c r="H123" s="6">
+        <v>61.732999999999997</v>
       </c>
       <c r="I123" s="6">
         <v>38048.1</v>
@@ -10587,8 +10587,8 @@
       <c r="G124" s="6">
         <v>1957</v>
       </c>
-      <c r="H124" s="7">
-        <v>-3.4500000000000028</v>
+      <c r="H124" s="6">
+        <v>61.77</v>
       </c>
       <c r="I124" s="6">
         <v>38349.800000000003</v>
@@ -10662,8 +10662,8 @@
       <c r="G125" s="6">
         <v>1966.6</v>
       </c>
-      <c r="H125" s="7">
-        <v>-3.4500000000000028</v>
+      <c r="H125" s="6">
+        <v>61.823999999999998</v>
       </c>
       <c r="I125" s="6">
         <v>38637.9</v>
@@ -10737,8 +10737,8 @@
       <c r="G126" s="6">
         <v>1663.6</v>
       </c>
-      <c r="H126" s="7">
-        <v>0.95000000000000284</v>
+      <c r="H126" s="6">
+        <v>66.173000000000002</v>
       </c>
       <c r="I126" s="6">
         <v>30652.9</v>
@@ -10812,8 +10812,8 @@
       <c r="G127" s="6">
         <v>1672.7</v>
       </c>
-      <c r="H127" s="7">
-        <v>0.95000000000000284</v>
+      <c r="H127" s="6">
+        <v>66.2</v>
       </c>
       <c r="I127" s="6">
         <v>30887.200000000001</v>
@@ -10887,8 +10887,8 @@
       <c r="G128" s="6">
         <v>1683.5</v>
       </c>
-      <c r="H128" s="7">
-        <v>1.0499999999999972</v>
+      <c r="H128" s="6">
+        <v>66.260000000000005</v>
       </c>
       <c r="I128" s="6">
         <v>31116.3</v>
@@ -10962,8 +10962,8 @@
       <c r="G129" s="6">
         <v>1693.4</v>
       </c>
-      <c r="H129" s="7">
-        <v>1.0499999999999972</v>
+      <c r="H129" s="6">
+        <v>66.269000000000005</v>
       </c>
       <c r="I129" s="6">
         <v>31341.9</v>
@@ -11037,8 +11037,8 @@
       <c r="G130" s="6">
         <v>1701.2</v>
       </c>
-      <c r="H130" s="7">
-        <v>0.95000000000000284</v>
+      <c r="H130" s="6">
+        <v>66.180000000000007</v>
       </c>
       <c r="I130" s="6">
         <v>31565.1</v>
@@ -11112,8 +11112,8 @@
       <c r="G131" s="6">
         <v>1709</v>
       </c>
-      <c r="H131" s="7">
-        <v>0.84999999999999432</v>
+      <c r="H131" s="6">
+        <v>66.064999999999998</v>
       </c>
       <c r="I131" s="6">
         <v>31787.599999999999</v>
@@ -11187,8 +11187,8 @@
       <c r="G132" s="6">
         <v>1717.1</v>
       </c>
-      <c r="H132" s="7">
-        <v>0.65000000000000568</v>
+      <c r="H132" s="6">
+        <v>65.933000000000007</v>
       </c>
       <c r="I132" s="6">
         <v>32010.9</v>
@@ -11262,8 +11262,8 @@
       <c r="G133" s="6">
         <v>1725.6</v>
       </c>
-      <c r="H133" s="7">
-        <v>0.54999999999999716</v>
+      <c r="H133" s="6">
+        <v>65.778000000000006</v>
       </c>
       <c r="I133" s="6">
         <v>32235.1</v>
@@ -11337,8 +11337,8 @@
       <c r="G134" s="6">
         <v>1734.8</v>
       </c>
-      <c r="H134" s="7">
-        <v>0.34999999999999432</v>
+      <c r="H134" s="6">
+        <v>65.593999999999994</v>
       </c>
       <c r="I134" s="6">
         <v>32462.400000000001</v>
@@ -11412,8 +11412,8 @@
       <c r="G135" s="6">
         <v>1744.5</v>
       </c>
-      <c r="H135" s="7">
-        <v>0.15000000000000568</v>
+      <c r="H135" s="6">
+        <v>65.373000000000005</v>
       </c>
       <c r="I135" s="6">
         <v>32697</v>
@@ -11487,8 +11487,8 @@
       <c r="G136" s="6">
         <v>1754.7</v>
       </c>
-      <c r="H136" s="7">
-        <v>-0.15000000000000568</v>
+      <c r="H136" s="6">
+        <v>65.096999999999994</v>
       </c>
       <c r="I136" s="6">
         <v>32936.5</v>
@@ -11562,8 +11562,8 @@
       <c r="G137" s="6">
         <v>1765.8</v>
       </c>
-      <c r="H137" s="7">
-        <v>-0.45000000000000284</v>
+      <c r="H137" s="6">
+        <v>64.783000000000001</v>
       </c>
       <c r="I137" s="6">
         <v>33184.300000000003</v>
@@ -11637,8 +11637,8 @@
       <c r="G138" s="6">
         <v>1777.9</v>
       </c>
-      <c r="H138" s="7">
-        <v>-0.84999999999999432</v>
+      <c r="H138" s="6">
+        <v>64.424000000000007</v>
       </c>
       <c r="I138" s="6">
         <v>33446.699999999997</v>
@@ -11712,8 +11712,8 @@
       <c r="G139" s="6">
         <v>1790.6</v>
       </c>
-      <c r="H139" s="7">
-        <v>-1.25</v>
+      <c r="H139" s="6">
+        <v>64.042000000000002</v>
       </c>
       <c r="I139" s="6">
         <v>33719.699999999997</v>
@@ -11787,8 +11787,8 @@
       <c r="G140" s="6">
         <v>1803.5</v>
       </c>
-      <c r="H140" s="7">
-        <v>-1.5499999999999972</v>
+      <c r="H140" s="6">
+        <v>63.66</v>
       </c>
       <c r="I140" s="6">
         <v>34002.1</v>
@@ -11862,8 +11862,8 @@
       <c r="G141" s="6">
         <v>1817.1</v>
       </c>
-      <c r="H141" s="7">
-        <v>-1.9500000000000028</v>
+      <c r="H141" s="6">
+        <v>63.262</v>
       </c>
       <c r="I141" s="6">
         <v>34297.199999999997</v>
@@ -11937,8 +11937,8 @@
       <c r="G142" s="6">
         <v>1831.1</v>
       </c>
-      <c r="H142" s="7">
-        <v>-2.3500000000000014</v>
+      <c r="H142" s="6">
+        <v>62.865000000000002</v>
       </c>
       <c r="I142" s="6">
         <v>34598.699999999997</v>
@@ -12012,8 +12012,8 @@
       <c r="G143" s="6">
         <v>1844.5</v>
       </c>
-      <c r="H143" s="7">
-        <v>-2.75</v>
+      <c r="H143" s="6">
+        <v>62.491999999999997</v>
       </c>
       <c r="I143" s="6">
         <v>34905.599999999999</v>
@@ -12087,8 +12087,8 @@
       <c r="G144" s="6">
         <v>1855.9</v>
       </c>
-      <c r="H144" s="7">
-        <v>-3.0499999999999972</v>
+      <c r="H144" s="6">
+        <v>62.183</v>
       </c>
       <c r="I144" s="6">
         <v>35214.9</v>
@@ -12162,8 +12162,8 @@
       <c r="G145" s="6">
         <v>1866.3</v>
       </c>
-      <c r="H145" s="7">
-        <v>-3.3500000000000014</v>
+      <c r="H145" s="6">
+        <v>61.921999999999997</v>
       </c>
       <c r="I145" s="6">
         <v>35527.699999999997</v>
@@ -12237,8 +12237,8 @@
       <c r="G146" s="6">
         <v>1875.8</v>
       </c>
-      <c r="H146" s="7">
-        <v>-3.5499999999999972</v>
+      <c r="H146" s="6">
+        <v>61.707999999999998</v>
       </c>
       <c r="I146" s="6">
         <v>35835.800000000003</v>
@@ -12312,8 +12312,8 @@
       <c r="G147" s="6">
         <v>1884.7</v>
       </c>
-      <c r="H147" s="7">
-        <v>-3.75</v>
+      <c r="H147" s="6">
+        <v>61.539000000000001</v>
       </c>
       <c r="I147" s="6">
         <v>36142.800000000003</v>
@@ -12387,8 +12387,8 @@
       <c r="G148" s="6">
         <v>1893.8</v>
       </c>
-      <c r="H148" s="7">
-        <v>-3.8500000000000014</v>
+      <c r="H148" s="6">
+        <v>61.404000000000003</v>
       </c>
       <c r="I148" s="6">
         <v>36450.699999999997</v>
@@ -12462,8 +12462,8 @@
       <c r="G149" s="6">
         <v>1902.6</v>
       </c>
-      <c r="H149" s="7">
-        <v>-3.9500000000000028</v>
+      <c r="H149" s="6">
+        <v>61.313000000000002</v>
       </c>
       <c r="I149" s="6">
         <v>36743.599999999999</v>
@@ -12537,8 +12537,8 @@
       <c r="G150" s="6">
         <v>1911.4</v>
       </c>
-      <c r="H150" s="7">
-        <v>-4.0499999999999972</v>
+      <c r="H150" s="6">
+        <v>61.246000000000002</v>
       </c>
       <c r="I150" s="6">
         <v>37041.800000000003</v>
@@ -12612,8 +12612,8 @@
       <c r="G151" s="6">
         <v>1920.1</v>
       </c>
-      <c r="H151" s="7">
-        <v>-4.0499999999999972</v>
+      <c r="H151" s="6">
+        <v>61.2</v>
       </c>
       <c r="I151" s="6">
         <v>37331.4</v>
@@ -12687,8 +12687,8 @@
       <c r="G152" s="6">
         <v>1928.8</v>
       </c>
-      <c r="H152" s="7">
-        <v>-4.0499999999999972</v>
+      <c r="H152" s="6">
+        <v>61.188000000000002</v>
       </c>
       <c r="I152" s="6">
         <v>37609.9</v>
@@ -12762,8 +12762,8 @@
       <c r="G153" s="6">
         <v>1937.6</v>
       </c>
-      <c r="H153" s="7">
-        <v>-4.0499999999999972</v>
+      <c r="H153" s="6">
+        <v>61.194000000000003</v>
       </c>
       <c r="I153" s="6">
         <v>37894.300000000003</v>
@@ -12837,8 +12837,8 @@
       <c r="G154" s="6">
         <v>1946.4</v>
       </c>
-      <c r="H154" s="7">
-        <v>-4.0499999999999972</v>
+      <c r="H154" s="6">
+        <v>61.22</v>
       </c>
       <c r="I154" s="6">
         <v>38165.599999999999</v>
@@ -12912,8 +12912,8 @@
       <c r="G155" s="6">
         <v>1955</v>
       </c>
-      <c r="H155" s="7">
-        <v>-3.9500000000000028</v>
+      <c r="H155" s="6">
+        <v>61.262999999999998</v>
       </c>
       <c r="I155" s="6">
         <v>38429.9</v>
@@ -12987,8 +12987,8 @@
       <c r="G156" s="6">
         <v>1963.9</v>
       </c>
-      <c r="H156" s="7">
-        <v>-3.9500000000000028</v>
+      <c r="H156" s="6">
+        <v>61.323999999999998</v>
       </c>
       <c r="I156" s="6">
         <v>38697.699999999997</v>
@@ -13062,8 +13062,8 @@
       <c r="G157" s="6">
         <v>1662.53</v>
       </c>
-      <c r="H157" s="7">
-        <v>0.68999999999999773</v>
+      <c r="H157" s="6">
+        <v>65.936999999999998</v>
       </c>
       <c r="I157" s="6">
         <v>30683.1</v>
@@ -13137,8 +13137,8 @@
       <c r="G158" s="6">
         <v>1672.29</v>
       </c>
-      <c r="H158" s="7">
-        <v>0.70999999999999375</v>
+      <c r="H158" s="6">
+        <v>65.962000000000003</v>
       </c>
       <c r="I158" s="6">
         <v>30927.9</v>
@@ -13212,8 +13212,8 @@
       <c r="G159" s="6">
         <v>1682.06</v>
       </c>
-      <c r="H159" s="7">
-        <v>0.71999999999999886</v>
+      <c r="H159" s="6">
+        <v>65.965000000000003</v>
       </c>
       <c r="I159" s="6">
         <v>31165.7</v>
@@ -13287,8 +13287,8 @@
       <c r="G160" s="6">
         <v>1693.81</v>
       </c>
-      <c r="H160" s="7">
-        <v>0.76000000000000512</v>
+      <c r="H160" s="6">
+        <v>66.013999999999996</v>
       </c>
       <c r="I160" s="6">
         <v>31399.9</v>
@@ -13362,8 +13362,8 @@
       <c r="G161" s="6">
         <v>1703.85</v>
       </c>
-      <c r="H161" s="7">
-        <v>0.73000000000000398</v>
+      <c r="H161" s="6">
+        <v>65.977999999999994</v>
       </c>
       <c r="I161" s="6">
         <v>31632.2</v>
@@ -13437,8 +13437,8 @@
       <c r="G162" s="6">
         <v>1712.33</v>
       </c>
-      <c r="H162" s="7">
-        <v>0.60999999999999943</v>
+      <c r="H162" s="6">
+        <v>65.86</v>
       </c>
       <c r="I162" s="6">
         <v>31863.3</v>
@@ -13512,8 +13512,8 @@
       <c r="G163" s="6">
         <v>1721.06</v>
       </c>
-      <c r="H163" s="7">
-        <v>0.45999999999999375</v>
+      <c r="H163" s="6">
+        <v>65.712000000000003</v>
       </c>
       <c r="I163" s="6">
         <v>32094.5</v>
@@ -13587,8 +13587,8 @@
       <c r="G164" s="6">
         <v>1730.39</v>
       </c>
-      <c r="H164" s="7">
-        <v>0.29000000000000625</v>
+      <c r="H164" s="6">
+        <v>65.537000000000006</v>
       </c>
       <c r="I164" s="6">
         <v>32327</v>
@@ -13662,8 +13662,8 @@
       <c r="G165" s="6">
         <v>1740.41</v>
       </c>
-      <c r="H165" s="7">
-        <v>7.9999999999998295E-2</v>
+      <c r="H165" s="6">
+        <v>65.331999999999994</v>
       </c>
       <c r="I165" s="6">
         <v>32565</v>
@@ -13737,8 +13737,8 @@
       <c r="G166" s="6">
         <v>1751.44</v>
       </c>
-      <c r="H166" s="7">
-        <v>-0.17000000000000171</v>
+      <c r="H166" s="6">
+        <v>65.084000000000003</v>
       </c>
       <c r="I166" s="6">
         <v>32808.699999999997</v>
@@ -13812,8 +13812,8 @@
       <c r="G167" s="6">
         <v>1763.08</v>
       </c>
-      <c r="H167" s="7">
-        <v>-0.45000000000000284</v>
+      <c r="H167" s="6">
+        <v>64.796000000000006</v>
       </c>
       <c r="I167" s="6">
         <v>33057.300000000003</v>
@@ -13887,8 +13887,8 @@
       <c r="G168" s="6">
         <v>1775.63</v>
       </c>
-      <c r="H168" s="7">
-        <v>-0.79999999999999716</v>
+      <c r="H168" s="6">
+        <v>64.445999999999998</v>
       </c>
       <c r="I168" s="6">
         <v>33319.599999999999</v>
@@ -13962,8 +13962,8 @@
       <c r="G169" s="6">
         <v>1788.58</v>
       </c>
-      <c r="H169" s="7">
-        <v>-1.1800000000000068</v>
+      <c r="H169" s="6">
+        <v>64.069000000000003</v>
       </c>
       <c r="I169" s="6">
         <v>33593.599999999999</v>
@@ -14037,8 +14037,8 @@
       <c r="G170" s="6">
         <v>1801.62</v>
       </c>
-      <c r="H170" s="7">
-        <v>-1.5700000000000003</v>
+      <c r="H170" s="6">
+        <v>63.683</v>
       </c>
       <c r="I170" s="6">
         <v>33874.400000000001</v>
@@ -14112,8 +14112,8 @@
       <c r="G171" s="6">
         <v>1815.15</v>
       </c>
-      <c r="H171" s="7">
-        <v>-1.9699999999999989</v>
+      <c r="H171" s="6">
+        <v>63.274999999999999</v>
       </c>
       <c r="I171" s="6">
         <v>34167.5</v>
@@ -14187,8 +14187,8 @@
       <c r="G172" s="6">
         <v>1829</v>
       </c>
-      <c r="H172" s="7">
-        <v>-2.3900000000000006</v>
+      <c r="H172" s="6">
+        <v>62.860999999999997</v>
       </c>
       <c r="I172" s="6">
         <v>34467.800000000003</v>
@@ -14262,8 +14262,8 @@
       <c r="G173" s="6">
         <v>1842.24</v>
       </c>
-      <c r="H173" s="7">
-        <v>-2.7700000000000031</v>
+      <c r="H173" s="6">
+        <v>62.481000000000002</v>
       </c>
       <c r="I173" s="6">
         <v>34771.4</v>
@@ -14337,8 +14337,8 @@
       <c r="G174" s="6">
         <v>1853.77</v>
       </c>
-      <c r="H174" s="7">
-        <v>-3.0799999999999983</v>
+      <c r="H174" s="6">
+        <v>62.170999999999999</v>
       </c>
       <c r="I174" s="6">
         <v>35077</v>
@@ -14412,8 +14412,8 @@
       <c r="G175" s="6">
         <v>1864.08</v>
       </c>
-      <c r="H175" s="7">
-        <v>-3.3400000000000034</v>
+      <c r="H175" s="6">
+        <v>61.905000000000001</v>
       </c>
       <c r="I175" s="6">
         <v>35385.800000000003</v>
@@ -14487,8 +14487,8 @@
       <c r="G176" s="6">
         <v>1873.28</v>
       </c>
-      <c r="H176" s="7">
-        <v>-3.5700000000000003</v>
+      <c r="H176" s="6">
+        <v>61.677</v>
       </c>
       <c r="I176" s="6">
         <v>35690.300000000003</v>
@@ -14562,8 +14562,8 @@
       <c r="G177" s="6">
         <v>1881.63</v>
       </c>
-      <c r="H177" s="7">
-        <v>-3.759999999999998</v>
+      <c r="H177" s="6">
+        <v>61.484999999999999</v>
       </c>
       <c r="I177" s="6">
         <v>35990.199999999997</v>
@@ -14637,8 +14637,8 @@
       <c r="G178" s="6">
         <v>1889.77</v>
       </c>
-      <c r="H178" s="7">
-        <v>-3.9299999999999997</v>
+      <c r="H178" s="6">
+        <v>61.316000000000003</v>
       </c>
       <c r="I178" s="6">
         <v>36293.9</v>
@@ -14712,8 +14712,8 @@
       <c r="G179" s="6">
         <v>1897.59</v>
       </c>
-      <c r="H179" s="7">
-        <v>-4.0600000000000023</v>
+      <c r="H179" s="6">
+        <v>61.185000000000002</v>
       </c>
       <c r="I179" s="6">
         <v>36579.699999999997</v>
@@ -14787,8 +14787,8 @@
       <c r="G180" s="6">
         <v>1905.51</v>
       </c>
-      <c r="H180" s="7">
-        <v>-4.1599999999999966</v>
+      <c r="H180" s="6">
+        <v>61.085999999999999</v>
       </c>
       <c r="I180" s="6">
         <v>36869.4</v>
@@ -14862,8 +14862,8 @@
       <c r="G181" s="6">
         <v>1913.67</v>
       </c>
-      <c r="H181" s="7">
-        <v>-4.2299999999999969</v>
+      <c r="H181" s="6">
+        <v>61.02</v>
       </c>
       <c r="I181" s="6">
         <v>37154</v>
@@ -14937,8 +14937,8 @@
       <c r="G182" s="6">
         <v>1921.58</v>
       </c>
-      <c r="H182" s="7">
-        <v>-4.2700000000000031</v>
+      <c r="H182" s="6">
+        <v>60.981000000000002</v>
       </c>
       <c r="I182" s="6">
         <v>37422.1</v>
@@ -15012,8 +15012,8 @@
       <c r="G183" s="6">
         <v>1929.59</v>
       </c>
-      <c r="H183" s="7">
-        <v>-4.2899999999999991</v>
+      <c r="H183" s="6">
+        <v>60.957000000000001</v>
       </c>
       <c r="I183" s="6">
         <v>37696</v>
@@ -15087,8 +15087,8 @@
       <c r="G184" s="6">
         <v>1937.77</v>
       </c>
-      <c r="H184" s="7">
-        <v>-4.2899999999999991</v>
+      <c r="H184" s="6">
+        <v>60.96</v>
       </c>
       <c r="I184" s="6">
         <v>37960.6</v>
@@ -15162,8 +15162,8 @@
       <c r="G185" s="6">
         <v>1945.94</v>
       </c>
-      <c r="H185" s="7">
-        <v>-4.259999999999998</v>
+      <c r="H185" s="6">
+        <v>60.988999999999997</v>
       </c>
       <c r="I185" s="6">
         <v>38213.599999999999</v>
@@ -15237,8 +15237,8 @@
       <c r="G186" s="6">
         <v>1954.2</v>
       </c>
-      <c r="H186" s="7">
-        <v>-4.2199999999999989</v>
+      <c r="H186" s="6">
+        <v>61.030999999999999</v>
       </c>
       <c r="I186" s="6">
         <v>38471.699999999997</v>
@@ -15312,8 +15312,8 @@
       <c r="G187" s="6">
         <v>1962.49</v>
       </c>
-      <c r="H187" s="7">
-        <v>-4.1599999999999966</v>
+      <c r="H187" s="6">
+        <v>61.085000000000001</v>
       </c>
       <c r="I187" s="6">
         <v>38722.199999999997</v>
@@ -15366,6 +15366,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -15373,8 +15374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B8FE5DC-F2F0-4529-A116-7170BC86971E}">
   <dimension ref="A1:M188"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
sofia | angle floating | fix
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/datasets/Stability/SSS_Sofia_Pantokarens_Angle_HydrostaticCurves.xlsx
+++ b/assets/fleet/9245263_sofia/datasets/Stability/SSS_Sofia_Pantokarens_Angle_HydrostaticCurves.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD9673A-310A-470A-93C1-B196742D1A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE42845-9353-4BBA-918F-AF3CC13DC3A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Angle" sheetId="1" r:id="rId1"/>
@@ -600,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,7 +636,7 @@
         <v>50.1</v>
       </c>
       <c r="D2" s="2">
-        <v>80</v>
+        <v>80.654599999999988</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -650,7 +650,7 @@
         <v>41.8</v>
       </c>
       <c r="D3" s="2">
-        <v>74</v>
+        <v>74.654599999999988</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -664,7 +664,7 @@
         <v>35.1</v>
       </c>
       <c r="D4" s="2">
-        <v>68.2</v>
+        <v>68.854600000000005</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -678,7 +678,7 @@
         <v>28.7</v>
       </c>
       <c r="D5" s="2">
-        <v>62.4</v>
+        <v>63.054599999999994</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -692,7 +692,7 @@
         <v>22.4</v>
       </c>
       <c r="D6" s="2">
-        <v>57</v>
+        <v>57.654599999999995</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -706,7 +706,7 @@
         <v>15.3</v>
       </c>
       <c r="D7" s="2">
-        <v>51.3</v>
+        <v>51.954599999999992</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -720,7 +720,7 @@
         <v>11.3</v>
       </c>
       <c r="D8" s="2">
-        <v>48.2</v>
+        <v>48.854599999999998</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -734,7 +734,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="D9" s="2">
-        <v>45.4</v>
+        <v>46.054599999999994</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -748,7 +748,7 @@
         <v>50.6</v>
       </c>
       <c r="D10" s="2">
-        <v>80.2</v>
+        <v>76.578000000000003</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -762,7 +762,7 @@
         <v>42.1</v>
       </c>
       <c r="D11" s="2">
-        <v>74.099999999999994</v>
+        <v>70.578000000000003</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -776,7 +776,7 @@
         <v>35.299999999999997</v>
       </c>
       <c r="D12" s="2">
-        <v>68.400000000000006</v>
+        <v>64.777999999999992</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -790,7 +790,7 @@
         <v>29.1</v>
       </c>
       <c r="D13" s="2">
-        <v>62.8</v>
+        <v>58.977999999999994</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -804,7 +804,7 @@
         <v>22.6</v>
       </c>
       <c r="D14" s="2">
-        <v>57.3</v>
+        <v>53.577999999999996</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -818,7 +818,7 @@
         <v>15.6</v>
       </c>
       <c r="D15" s="2">
-        <v>51.5</v>
+        <v>47.877999999999993</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -832,7 +832,7 @@
         <v>11.7</v>
       </c>
       <c r="D16" s="2">
-        <v>48.4</v>
+        <v>44.777999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -846,7 +846,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="D17" s="1">
-        <v>45.8</v>
+        <v>41.977999999999994</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -860,7 +860,7 @@
         <v>50.95</v>
       </c>
       <c r="D18" s="2">
-        <v>80.400000000000006</v>
+        <v>79.754599999999982</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -874,7 +874,7 @@
         <v>42.41</v>
       </c>
       <c r="D19" s="2">
-        <v>74.2</v>
+        <v>73.754599999999982</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -888,7 +888,7 @@
         <v>35.4</v>
       </c>
       <c r="D20" s="2">
-        <v>68.44</v>
+        <v>67.954599999999999</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -902,7 +902,7 @@
         <v>29.2</v>
       </c>
       <c r="D21" s="2">
-        <v>62.96</v>
+        <v>62.154599999999995</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -916,7 +916,7 @@
         <v>22.6</v>
       </c>
       <c r="D22" s="2">
-        <v>57.25</v>
+        <v>56.754599999999996</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -930,7 +930,7 @@
         <v>15.7</v>
       </c>
       <c r="D23" s="2">
-        <v>51.65</v>
+        <v>51.054599999999994</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -944,7 +944,7 @@
         <v>12.1</v>
       </c>
       <c r="D24" s="2">
-        <v>48.79</v>
+        <v>47.954599999999999</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -958,7 +958,7 @@
         <v>8.44</v>
       </c>
       <c r="D25" s="2">
-        <v>45.87</v>
+        <v>45.154599999999995</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -972,7 +972,7 @@
         <v>51.26</v>
       </c>
       <c r="D26" s="2">
-        <v>80.599999999999994</v>
+        <v>78.928399999999996</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -986,7 +986,7 @@
         <v>42.85</v>
       </c>
       <c r="D27" s="2">
-        <v>74.5</v>
+        <v>72.928399999999996</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1000,7 +1000,7 @@
         <v>35.42</v>
       </c>
       <c r="D28" s="2">
-        <v>68.5</v>
+        <v>67.128399999999999</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1014,7 +1014,7 @@
         <v>29.34</v>
       </c>
       <c r="D29" s="2">
-        <v>63.2</v>
+        <v>61.328399999999995</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1028,7 +1028,7 @@
         <v>22.56</v>
       </c>
       <c r="D30" s="2">
-        <v>57.3</v>
+        <v>55.928399999999996</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1042,7 +1042,7 @@
         <v>15.92</v>
       </c>
       <c r="D31" s="2">
-        <v>51.9</v>
+        <v>50.228399999999993</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1056,7 +1056,7 @@
         <v>12.39</v>
       </c>
       <c r="D32" s="2">
-        <v>49.1</v>
+        <v>47.128399999999999</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1070,7 +1070,7 @@
         <v>8.73</v>
       </c>
       <c r="D33" s="2">
-        <v>46.07</v>
+        <v>44.328399999999995</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1084,7 +1084,7 @@
         <v>51.58</v>
       </c>
       <c r="D34" s="2">
-        <v>80.8</v>
+        <v>77.099999999999994</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1098,7 +1098,7 @@
         <v>43.42</v>
       </c>
       <c r="D35" s="2">
-        <v>74.900000000000006</v>
+        <v>71.099999999999994</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1112,7 +1112,7 @@
         <v>36.18</v>
       </c>
       <c r="D36" s="2">
-        <v>69.2</v>
+        <v>65.3</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1126,7 +1126,7 @@
         <v>29.86</v>
       </c>
       <c r="D37" s="2">
-        <v>63.9</v>
+        <v>59.499999999999993</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1140,7 +1140,7 @@
         <v>23.85</v>
       </c>
       <c r="D38" s="2">
-        <v>58.6</v>
+        <v>54.099999999999994</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1154,7 +1154,7 @@
         <v>16.63</v>
       </c>
       <c r="D39" s="2">
-        <v>52.5</v>
+        <v>48.399999999999991</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1168,7 +1168,7 @@
         <v>13.22</v>
       </c>
       <c r="D40" s="2">
-        <v>49.8</v>
+        <v>45.3</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1182,7 +1182,7 @@
         <v>9.24</v>
       </c>
       <c r="D41" s="2">
-        <v>46.52</v>
+        <v>42.499999999999993</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1196,7 +1196,7 @@
         <v>51.42</v>
       </c>
       <c r="D42" s="2">
-        <v>80.900000000000006</v>
+        <v>76.199999999999989</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1210,7 +1210,7 @@
         <v>43.71</v>
       </c>
       <c r="D43" s="2">
-        <v>75.099999999999994</v>
+        <v>70.199999999999989</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1224,7 +1224,7 @@
         <v>36.78</v>
       </c>
       <c r="D44" s="2">
-        <v>69.7</v>
+        <v>64.400000000000006</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1238,7 +1238,7 @@
         <v>30.82</v>
       </c>
       <c r="D45" s="2">
-        <v>64.8</v>
+        <v>58.599999999999994</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1252,7 +1252,7 @@
         <v>23.59</v>
       </c>
       <c r="D46" s="2">
-        <v>58.4</v>
+        <v>53.199999999999996</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1266,7 +1266,7 @@
         <v>17.329999999999998</v>
       </c>
       <c r="D47" s="2">
-        <v>53.2</v>
+        <v>47.499999999999993</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1280,7 +1280,7 @@
         <v>11.5</v>
       </c>
       <c r="D48" s="2">
-        <v>49</v>
+        <v>44.4</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1294,7 +1294,7 @@
         <v>9.33</v>
       </c>
       <c r="D49" s="2">
-        <v>46.61</v>
+        <v>41.599999999999994</v>
       </c>
     </row>
   </sheetData>
@@ -1307,7 +1307,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A4FC80-BF2A-45A2-A621-AB74F1039367}">
   <dimension ref="A1:Y187"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
sofia | angle | bug fix
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/datasets/Stability/SSS_Sofia_Pantokarens_Angle_HydrostaticCurves.xlsx
+++ b/assets/fleet/9245263_sofia/datasets/Stability/SSS_Sofia_Pantokarens_Angle_HydrostaticCurves.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A344FF7B-D6ED-494F-BE4B-A4956BB61348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A7BD25F-E0FC-445C-B233-6AF3D2372785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Angle" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1767" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1761" uniqueCount="31">
   <si>
     <t>trim [m]</t>
   </si>
@@ -115,22 +115,16 @@
     <t>Крен/Heel</t>
   </si>
   <si>
-    <t>trim</t>
+    <t>trim  [m]</t>
   </si>
   <si>
-    <t xml:space="preserve"> [m]</t>
+    <t>draft  [m]</t>
   </si>
   <si>
-    <t>deckAngle</t>
+    <t>floodAngle [degree]</t>
   </si>
   <si>
-    <t>draft</t>
-  </si>
-  <si>
-    <t>[degree]</t>
-  </si>
-  <si>
-    <t>floodAngle</t>
+    <t>deckAngle [degree]</t>
   </si>
 </sst>
 </file>
@@ -663,10 +657,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Лист1"/>
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:F11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,55 +674,55 @@
         <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>31</v>
+      <c r="A2" s="4">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C2" s="1">
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="C3" s="1">
-        <v>86</v>
-      </c>
+      <c r="A3" s="1">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="C3" s="2">
+        <v>80.654600000000002</v>
+      </c>
+      <c r="D3" s="24"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0</v>
       </c>
       <c r="B4" s="2">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="C4" s="2">
-        <v>80.654600000000002</v>
-      </c>
-      <c r="D4" s="24"/>
+        <v>74.654599999999988</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0</v>
       </c>
       <c r="B5" s="2">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="C5" s="2">
-        <v>74.654599999999988</v>
+        <v>68.854600000000005</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -736,83 +730,84 @@
         <v>0</v>
       </c>
       <c r="B6" s="2">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="C6" s="2">
-        <v>68.854600000000005</v>
-      </c>
+        <v>63.054599999999994</v>
+      </c>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0</v>
       </c>
       <c r="B7" s="2">
-        <v>5.5</v>
+        <v>6.5</v>
       </c>
       <c r="C7" s="2">
-        <v>63.054599999999994</v>
-      </c>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
+        <v>57.654599999999995</v>
+      </c>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>0</v>
       </c>
       <c r="B8" s="2">
-        <v>6.5</v>
+        <v>7.5</v>
       </c>
       <c r="C8" s="2">
-        <v>57.654599999999995</v>
-      </c>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
+        <v>51.954599999999992</v>
+      </c>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>0</v>
       </c>
       <c r="B9" s="2">
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="C9" s="2">
-        <v>51.954599999999992</v>
-      </c>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
+        <v>48.854599999999998</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>0</v>
       </c>
-      <c r="B10" s="2">
-        <v>8</v>
+      <c r="B10" s="3">
+        <v>8.5</v>
       </c>
       <c r="C10" s="2">
-        <v>48.854599999999998</v>
+        <v>46.054599999999994</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>0</v>
+      <c r="A11" s="4">
+        <v>-0.16800000000000001</v>
       </c>
       <c r="B11" s="3">
-        <v>8.5</v>
+        <v>1.5</v>
       </c>
       <c r="C11" s="2">
-        <v>46.054599999999994</v>
+        <f>C2-(C2-C20)/0.4*0.168</f>
+        <v>85.602931999999996</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>-0.16800000000000001</v>
       </c>
-      <c r="B12" s="3">
-        <v>1.5</v>
+      <c r="B12" s="2">
+        <v>2.5</v>
       </c>
       <c r="C12" s="2">
-        <f>C3-(C3-C21)/0.4*0.168</f>
-        <v>85.602931999999996</v>
+        <f t="shared" ref="C12:C19" si="0">C3-(C3-C21)/0.4*0.168</f>
+        <v>80.276599999999988</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -820,11 +815,11 @@
         <v>-0.16800000000000001</v>
       </c>
       <c r="B13" s="2">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="C13" s="2">
-        <f t="shared" ref="C13:C20" si="0">C4-(C4-C22)/0.4*0.168</f>
-        <v>80.276599999999988</v>
+        <f t="shared" si="0"/>
+        <v>74.276599999999988</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -832,11 +827,11 @@
         <v>-0.16800000000000001</v>
       </c>
       <c r="B14" s="2">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="C14" s="2">
         <f t="shared" si="0"/>
-        <v>74.276599999999988</v>
+        <v>68.476600000000005</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -844,11 +839,11 @@
         <v>-0.16800000000000001</v>
       </c>
       <c r="B15" s="2">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="C15" s="2">
         <f t="shared" si="0"/>
-        <v>68.476600000000005</v>
+        <v>62.676599999999993</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -856,11 +851,11 @@
         <v>-0.16800000000000001</v>
       </c>
       <c r="B16" s="2">
-        <v>5.5</v>
+        <v>6.5</v>
       </c>
       <c r="C16" s="2">
         <f t="shared" si="0"/>
-        <v>62.676599999999993</v>
+        <v>57.276599999999995</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -868,11 +863,11 @@
         <v>-0.16800000000000001</v>
       </c>
       <c r="B17" s="2">
-        <v>6.5</v>
+        <v>7.5</v>
       </c>
       <c r="C17" s="2">
         <f t="shared" si="0"/>
-        <v>57.276599999999995</v>
+        <v>51.576599999999992</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -880,46 +875,45 @@
         <v>-0.16800000000000001</v>
       </c>
       <c r="B18" s="2">
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="C18" s="2">
         <f t="shared" si="0"/>
-        <v>51.576599999999992</v>
+        <v>48.476599999999998</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>-0.16800000000000001</v>
       </c>
-      <c r="B19" s="2">
-        <v>8</v>
+      <c r="B19" s="3">
+        <v>8.5</v>
       </c>
       <c r="C19" s="2">
         <f t="shared" si="0"/>
-        <v>48.476599999999998</v>
+        <v>45.676599999999993</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
-        <v>-0.16800000000000001</v>
+        <v>-0.4</v>
       </c>
       <c r="B20" s="3">
-        <v>8.5</v>
+        <v>1.5</v>
       </c>
       <c r="C20" s="2">
-        <f t="shared" si="0"/>
-        <v>45.676599999999993</v>
+        <v>85.054599999999979</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>-0.4</v>
       </c>
-      <c r="B21" s="3">
-        <v>1.5</v>
+      <c r="B21" s="2">
+        <v>2.5</v>
       </c>
       <c r="C21" s="2">
-        <v>85.054599999999979</v>
+        <v>79.754599999999982</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -927,10 +921,10 @@
         <v>-0.4</v>
       </c>
       <c r="B22" s="2">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="C22" s="2">
-        <v>79.754599999999982</v>
+        <v>73.754599999999982</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -938,10 +932,10 @@
         <v>-0.4</v>
       </c>
       <c r="B23" s="2">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="C23" s="2">
-        <v>73.754599999999982</v>
+        <v>67.954599999999999</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -949,10 +943,10 @@
         <v>-0.4</v>
       </c>
       <c r="B24" s="2">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="C24" s="2">
-        <v>67.954599999999999</v>
+        <v>62.154599999999995</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -960,10 +954,10 @@
         <v>-0.4</v>
       </c>
       <c r="B25" s="2">
-        <v>5.5</v>
+        <v>6.5</v>
       </c>
       <c r="C25" s="2">
-        <v>62.154599999999995</v>
+        <v>56.754599999999996</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -971,10 +965,10 @@
         <v>-0.4</v>
       </c>
       <c r="B26" s="2">
-        <v>6.5</v>
+        <v>7.5</v>
       </c>
       <c r="C26" s="2">
-        <v>56.754599999999996</v>
+        <v>51.054599999999994</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -982,43 +976,43 @@
         <v>-0.4</v>
       </c>
       <c r="B27" s="2">
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="C27" s="2">
-        <v>51.054599999999994</v>
+        <v>47.954599999999999</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>-0.4</v>
       </c>
-      <c r="B28" s="2">
-        <v>8</v>
+      <c r="B28" s="3">
+        <v>8.5</v>
       </c>
       <c r="C28" s="2">
-        <v>47.954599999999999</v>
+        <v>45.154599999999995</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
       <c r="B29" s="3">
-        <v>8.5</v>
+        <v>1.5</v>
       </c>
       <c r="C29" s="2">
-        <v>45.154599999999995</v>
+        <v>84.228399999999993</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>-0.8</v>
       </c>
-      <c r="B30" s="3">
-        <v>1.5</v>
+      <c r="B30" s="2">
+        <v>2.5</v>
       </c>
       <c r="C30" s="2">
-        <v>84.228399999999993</v>
+        <v>78.928399999999996</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1026,10 +1020,10 @@
         <v>-0.8</v>
       </c>
       <c r="B31" s="2">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="C31" s="2">
-        <v>78.928399999999996</v>
+        <v>72.928399999999996</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1037,10 +1031,10 @@
         <v>-0.8</v>
       </c>
       <c r="B32" s="2">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="C32" s="2">
-        <v>72.928399999999996</v>
+        <v>67.128399999999999</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1048,10 +1042,10 @@
         <v>-0.8</v>
       </c>
       <c r="B33" s="2">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="C33" s="2">
-        <v>67.128399999999999</v>
+        <v>61.328399999999995</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1059,10 +1053,10 @@
         <v>-0.8</v>
       </c>
       <c r="B34" s="2">
-        <v>5.5</v>
+        <v>6.5</v>
       </c>
       <c r="C34" s="2">
-        <v>61.328399999999995</v>
+        <v>55.928399999999996</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1070,10 +1064,10 @@
         <v>-0.8</v>
       </c>
       <c r="B35" s="2">
-        <v>6.5</v>
+        <v>7.5</v>
       </c>
       <c r="C35" s="2">
-        <v>55.928399999999996</v>
+        <v>50.228399999999993</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1081,43 +1075,43 @@
         <v>-0.8</v>
       </c>
       <c r="B36" s="2">
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="C36" s="2">
-        <v>50.228399999999993</v>
+        <v>47.128399999999999</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>-0.8</v>
       </c>
-      <c r="B37" s="2">
-        <v>8</v>
+      <c r="B37" s="3">
+        <v>8.5</v>
       </c>
       <c r="C37" s="2">
-        <v>47.128399999999999</v>
+        <v>44.328399999999995</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
-        <v>-0.8</v>
+        <v>-1.6</v>
       </c>
       <c r="B38" s="3">
-        <v>8.5</v>
+        <v>1.5</v>
       </c>
       <c r="C38" s="2">
-        <v>44.328399999999995</v>
+        <v>82.399999999999991</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>-1.6</v>
       </c>
-      <c r="B39" s="3">
-        <v>1.5</v>
+      <c r="B39" s="2">
+        <v>2.5</v>
       </c>
       <c r="C39" s="2">
-        <v>82.399999999999991</v>
+        <v>77.099999999999994</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1125,10 +1119,10 @@
         <v>-1.6</v>
       </c>
       <c r="B40" s="2">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="C40" s="2">
-        <v>77.099999999999994</v>
+        <v>71.099999999999994</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1136,10 +1130,10 @@
         <v>-1.6</v>
       </c>
       <c r="B41" s="2">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="C41" s="2">
-        <v>71.099999999999994</v>
+        <v>65.3</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1147,10 +1141,10 @@
         <v>-1.6</v>
       </c>
       <c r="B42" s="2">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="C42" s="2">
-        <v>65.3</v>
+        <v>59.499999999999993</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1158,10 +1152,10 @@
         <v>-1.6</v>
       </c>
       <c r="B43" s="2">
-        <v>5.5</v>
+        <v>6.5</v>
       </c>
       <c r="C43" s="2">
-        <v>59.499999999999993</v>
+        <v>54.099999999999994</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1169,10 +1163,10 @@
         <v>-1.6</v>
       </c>
       <c r="B44" s="2">
-        <v>6.5</v>
+        <v>7.5</v>
       </c>
       <c r="C44" s="2">
-        <v>54.099999999999994</v>
+        <v>48.399999999999991</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1180,43 +1174,43 @@
         <v>-1.6</v>
       </c>
       <c r="B45" s="2">
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="C45" s="2">
-        <v>48.399999999999991</v>
+        <v>45.3</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>-1.6</v>
       </c>
-      <c r="B46" s="2">
-        <v>8</v>
+      <c r="B46" s="3">
+        <v>8.5</v>
       </c>
       <c r="C46" s="2">
-        <v>45.3</v>
+        <v>42.499999999999993</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
       <c r="B47" s="3">
-        <v>8.5</v>
+        <v>1.5</v>
       </c>
       <c r="C47" s="2">
-        <v>42.499999999999993</v>
+        <v>81.499999999999986</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>-2</v>
       </c>
-      <c r="B48" s="3">
-        <v>1.5</v>
+      <c r="B48" s="2">
+        <v>2.5</v>
       </c>
       <c r="C48" s="2">
-        <v>81.499999999999986</v>
+        <v>76.199999999999989</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1224,10 +1218,10 @@
         <v>-2</v>
       </c>
       <c r="B49" s="2">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="C49" s="2">
-        <v>76.199999999999989</v>
+        <v>70.199999999999989</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1235,10 +1229,10 @@
         <v>-2</v>
       </c>
       <c r="B50" s="2">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="C50" s="2">
-        <v>70.199999999999989</v>
+        <v>64.400000000000006</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1246,10 +1240,10 @@
         <v>-2</v>
       </c>
       <c r="B51" s="2">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="C51" s="2">
-        <v>64.400000000000006</v>
+        <v>58.599999999999994</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1257,10 +1251,10 @@
         <v>-2</v>
       </c>
       <c r="B52" s="2">
-        <v>5.5</v>
+        <v>6.5</v>
       </c>
       <c r="C52" s="2">
-        <v>58.599999999999994</v>
+        <v>53.199999999999996</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1268,10 +1262,10 @@
         <v>-2</v>
       </c>
       <c r="B53" s="2">
-        <v>6.5</v>
+        <v>7.5</v>
       </c>
       <c r="C53" s="2">
-        <v>53.199999999999996</v>
+        <v>47.499999999999993</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1279,31 +1273,20 @@
         <v>-2</v>
       </c>
       <c r="B54" s="2">
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="C54" s="2">
-        <v>47.499999999999993</v>
+        <v>44.4</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>-2</v>
       </c>
-      <c r="B55" s="2">
-        <v>8</v>
+      <c r="B55" s="3">
+        <v>8.5</v>
       </c>
       <c r="C55" s="2">
-        <v>44.4</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="4">
-        <v>-2</v>
-      </c>
-      <c r="B56" s="3">
-        <v>8.5</v>
-      </c>
-      <c r="C56" s="2">
         <v>41.599999999999994</v>
       </c>
     </row>
@@ -17650,7 +17633,7 @@
   <dimension ref="A1:Z218"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26595,10 +26578,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DA40484-3319-4556-998F-B01A9379511C}">
-  <dimension ref="A1:F95"/>
+  <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E86" sqref="E86"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26613,21 +26596,21 @@
         <v>27</v>
       </c>
       <c r="B1" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>31</v>
+      <c r="A2" s="4">
+        <v>0</v>
+      </c>
+      <c r="B2" s="29">
+        <v>1.5</v>
+      </c>
+      <c r="C2" s="25">
+        <v>63.260329773536803</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -26635,33 +26618,33 @@
         <v>0</v>
       </c>
       <c r="B3" s="29">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="C3" s="25">
-        <v>63.260329773536803</v>
-      </c>
+        <v>59.407452976870999</v>
+      </c>
+      <c r="D3" s="24"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>0</v>
       </c>
-      <c r="B4" s="29">
-        <v>2</v>
+      <c r="B4" s="30">
+        <v>2.5365500000000001</v>
       </c>
       <c r="C4" s="25">
-        <v>59.407452976870999</v>
-      </c>
-      <c r="D4" s="24"/>
+        <v>55.211599999999997</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="1">
         <v>0</v>
       </c>
       <c r="B5" s="30">
-        <v>2.5365500000000001</v>
+        <v>2.9444400000000002</v>
       </c>
       <c r="C5" s="25">
-        <v>55.211599999999997</v>
+        <v>51.670400000000001</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -26669,60 +26652,60 @@
         <v>0</v>
       </c>
       <c r="B6" s="30">
-        <v>2.9444400000000002</v>
+        <v>3.7487900000000001</v>
       </c>
       <c r="C6" s="25">
-        <v>51.670400000000001</v>
-      </c>
+        <v>45.790599999999998</v>
+      </c>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0</v>
       </c>
       <c r="B7" s="30">
-        <v>3.7487900000000001</v>
+        <v>4.5529000000000002</v>
       </c>
       <c r="C7" s="25">
-        <v>45.790599999999998</v>
-      </c>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
+        <v>40.579099999999997</v>
+      </c>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>0</v>
       </c>
       <c r="B8" s="30">
-        <v>4.5529000000000002</v>
+        <v>5.3456299999999999</v>
       </c>
       <c r="C8" s="25">
-        <v>40.579099999999997</v>
-      </c>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
+        <v>36.436500000000002</v>
+      </c>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>0</v>
       </c>
       <c r="B9" s="30">
-        <v>5.3456299999999999</v>
+        <v>6.1493399999999996</v>
       </c>
       <c r="C9" s="25">
-        <v>36.436500000000002</v>
-      </c>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
+        <v>32.293999999999997</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>0</v>
       </c>
       <c r="B10" s="30">
-        <v>6.1493399999999996</v>
+        <v>7.34945</v>
       </c>
       <c r="C10" s="25">
-        <v>32.293999999999997</v>
+        <v>26.013400000000001</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -26730,32 +26713,32 @@
         <v>0</v>
       </c>
       <c r="B11" s="30">
-        <v>7.34945</v>
+        <v>8.1534300000000002</v>
       </c>
       <c r="C11" s="25">
-        <v>26.013400000000001</v>
+        <v>21.135899999999999</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>0</v>
       </c>
-      <c r="B12" s="30">
-        <v>8.1534300000000002</v>
+      <c r="B12" s="31">
+        <v>8.4728700000000003</v>
       </c>
       <c r="C12" s="25">
-        <v>21.135899999999999</v>
+        <v>19.064599999999999</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>0</v>
-      </c>
-      <c r="B13" s="31">
-        <v>8.4728700000000003</v>
+      <c r="A13" s="4">
+        <v>-0.16800000000000001</v>
+      </c>
+      <c r="B13" s="29">
+        <v>1.5</v>
       </c>
       <c r="C13" s="25">
-        <v>19.064599999999999</v>
+        <v>63.609406992035503</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -26763,21 +26746,21 @@
         <v>-0.16800000000000001</v>
       </c>
       <c r="B14" s="29">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="C14" s="25">
-        <v>63.609406992035503</v>
+        <v>59.769602357878</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>-0.16800000000000001</v>
       </c>
-      <c r="B15" s="29">
-        <v>2</v>
+      <c r="B15" s="30">
+        <v>2.5464600000000002</v>
       </c>
       <c r="C15" s="25">
-        <v>59.769602357878</v>
+        <v>55.767800000000001</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -26785,10 +26768,10 @@
         <v>-0.16800000000000001</v>
       </c>
       <c r="B16" s="30">
-        <v>2.5464600000000002</v>
+        <v>2.93363</v>
       </c>
       <c r="C16" s="25">
-        <v>55.767800000000001</v>
+        <v>52.120699999999999</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -26796,10 +26779,10 @@
         <v>-0.16800000000000001</v>
       </c>
       <c r="B17" s="30">
-        <v>2.93363</v>
+        <v>3.3429199999999999</v>
       </c>
       <c r="C17" s="25">
-        <v>52.120699999999999</v>
+        <v>48.985399999999998</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -26807,10 +26790,10 @@
         <v>-0.16800000000000001</v>
       </c>
       <c r="B18" s="30">
-        <v>3.3429199999999999</v>
+        <v>3.7632699999999999</v>
       </c>
       <c r="C18" s="25">
-        <v>48.985399999999998</v>
+        <v>46.17</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -26818,10 +26801,10 @@
         <v>-0.16800000000000001</v>
       </c>
       <c r="B19" s="30">
-        <v>3.7632699999999999</v>
+        <v>4.1615000000000002</v>
       </c>
       <c r="C19" s="25">
-        <v>46.17</v>
+        <v>43.482599999999998</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -26829,10 +26812,10 @@
         <v>-0.16800000000000001</v>
       </c>
       <c r="B20" s="30">
-        <v>4.1615000000000002</v>
+        <v>4.5597300000000001</v>
       </c>
       <c r="C20" s="25">
-        <v>43.482599999999998</v>
+        <v>41.051200000000001</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -26840,10 +26823,10 @@
         <v>-0.16800000000000001</v>
       </c>
       <c r="B21" s="30">
-        <v>4.5597300000000001</v>
+        <v>4.9690300000000001</v>
       </c>
       <c r="C21" s="25">
-        <v>41.051200000000001</v>
+        <v>38.811700000000002</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -26851,10 +26834,10 @@
         <v>-0.16800000000000001</v>
       </c>
       <c r="B22" s="30">
-        <v>4.9690300000000001</v>
+        <v>5.3672599999999999</v>
       </c>
       <c r="C22" s="25">
-        <v>38.811700000000002</v>
+        <v>36.764200000000002</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -26862,10 +26845,10 @@
         <v>-0.16800000000000001</v>
       </c>
       <c r="B23" s="30">
-        <v>5.3672599999999999</v>
+        <v>6.1526500000000004</v>
       </c>
       <c r="C23" s="25">
-        <v>36.764200000000002</v>
+        <v>32.7331</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -26873,10 +26856,10 @@
         <v>-0.16800000000000001</v>
       </c>
       <c r="B24" s="30">
-        <v>6.1526500000000004</v>
+        <v>6.9491199999999997</v>
       </c>
       <c r="C24" s="25">
-        <v>32.7331</v>
+        <v>28.638000000000002</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -26884,10 +26867,10 @@
         <v>-0.16800000000000001</v>
       </c>
       <c r="B25" s="30">
-        <v>6.9491199999999997</v>
+        <v>7.7455800000000004</v>
       </c>
       <c r="C25" s="25">
-        <v>28.638000000000002</v>
+        <v>24.158999999999999</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -26895,21 +26878,21 @@
         <v>-0.16800000000000001</v>
       </c>
       <c r="B26" s="30">
-        <v>7.7455800000000004</v>
+        <v>8.4867299999999997</v>
       </c>
       <c r="C26" s="25">
-        <v>24.158999999999999</v>
+        <v>19.552099999999999</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
-        <v>-0.16800000000000001</v>
-      </c>
-      <c r="B27" s="30">
-        <v>8.4867299999999997</v>
+        <v>-0.4</v>
+      </c>
+      <c r="B27" s="29">
+        <v>1.5</v>
       </c>
       <c r="C27" s="25">
-        <v>19.552099999999999</v>
+        <v>64.101699568578198</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -26917,21 +26900,21 @@
         <v>-0.4</v>
       </c>
       <c r="B28" s="29">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="C28" s="25">
-        <v>64.101699568578198</v>
+        <v>60.279946968360903</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>-0.4</v>
       </c>
-      <c r="B29" s="29">
-        <v>2</v>
+      <c r="B29" s="28">
+        <v>2.5425900000000001</v>
       </c>
       <c r="C29" s="25">
-        <v>60.279946968360903</v>
+        <v>56.512599999999999</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -26939,10 +26922,10 @@
         <v>-0.4</v>
       </c>
       <c r="B30" s="28">
-        <v>2.5425900000000001</v>
+        <v>2.9438599999999999</v>
       </c>
       <c r="C30" s="25">
-        <v>56.512599999999999</v>
+        <v>52.857100000000003</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -26950,10 +26933,10 @@
         <v>-0.4</v>
       </c>
       <c r="B31" s="28">
-        <v>2.9438599999999999</v>
+        <v>3.3563200000000002</v>
       </c>
       <c r="C31" s="25">
-        <v>52.857100000000003</v>
+        <v>49.579799999999999</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -26961,10 +26944,10 @@
         <v>-0.4</v>
       </c>
       <c r="B32" s="28">
-        <v>3.3563200000000002</v>
+        <v>3.7581799999999999</v>
       </c>
       <c r="C32" s="25">
-        <v>49.579799999999999</v>
+        <v>46.743699999999997</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -26972,10 +26955,10 @@
         <v>-0.4</v>
       </c>
       <c r="B33" s="28">
-        <v>3.7581799999999999</v>
+        <v>4.1491800000000003</v>
       </c>
       <c r="C33" s="25">
-        <v>46.743699999999997</v>
+        <v>43.970599999999997</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -26983,10 +26966,10 @@
         <v>-0.4</v>
       </c>
       <c r="B34" s="28">
-        <v>4.1491800000000003</v>
+        <v>4.5512699999999997</v>
       </c>
       <c r="C34" s="25">
-        <v>43.970599999999997</v>
+        <v>41.449599999999997</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -26994,10 +26977,10 @@
         <v>-0.4</v>
       </c>
       <c r="B35" s="28">
-        <v>4.5512699999999997</v>
+        <v>4.9644700000000004</v>
       </c>
       <c r="C35" s="25">
-        <v>41.449599999999997</v>
+        <v>39.180700000000002</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -27005,10 +26988,10 @@
         <v>-0.4</v>
       </c>
       <c r="B36" s="28">
-        <v>4.9644700000000004</v>
+        <v>5.36693</v>
       </c>
       <c r="C36" s="25">
-        <v>39.180700000000002</v>
+        <v>37.163899999999998</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -27016,10 +26999,10 @@
         <v>-0.4</v>
       </c>
       <c r="B37" s="28">
-        <v>5.36693</v>
+        <v>5.7584799999999996</v>
       </c>
       <c r="C37" s="25">
-        <v>37.163899999999998</v>
+        <v>35.147100000000002</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -27027,10 +27010,10 @@
         <v>-0.4</v>
       </c>
       <c r="B38" s="28">
-        <v>5.7584799999999996</v>
+        <v>6.1609400000000001</v>
       </c>
       <c r="C38" s="25">
-        <v>35.147100000000002</v>
+        <v>33.130299999999998</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -27038,10 +27021,10 @@
         <v>-0.4</v>
       </c>
       <c r="B39" s="28">
-        <v>6.1609400000000001</v>
+        <v>6.5524800000000001</v>
       </c>
       <c r="C39" s="25">
-        <v>33.130299999999998</v>
+        <v>31.113399999999999</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -27049,10 +27032,10 @@
         <v>-0.4</v>
       </c>
       <c r="B40" s="28">
-        <v>6.5524800000000001</v>
+        <v>6.9549500000000002</v>
       </c>
       <c r="C40" s="25">
-        <v>31.113399999999999</v>
+        <v>29.096599999999999</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -27060,10 +27043,10 @@
         <v>-0.4</v>
       </c>
       <c r="B41" s="28">
-        <v>6.9549500000000002</v>
+        <v>7.3464499999999999</v>
       </c>
       <c r="C41" s="25">
-        <v>29.096599999999999</v>
+        <v>27.0168</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -27071,10 +27054,10 @@
         <v>-0.4</v>
       </c>
       <c r="B42" s="28">
-        <v>7.3464499999999999</v>
+        <v>7.7486800000000002</v>
       </c>
       <c r="C42" s="25">
-        <v>27.0168</v>
+        <v>24.684899999999999</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -27082,32 +27065,32 @@
         <v>-0.4</v>
       </c>
       <c r="B43" s="28">
-        <v>7.7486800000000002</v>
+        <v>8.1399500000000007</v>
       </c>
       <c r="C43" s="25">
-        <v>24.684899999999999</v>
+        <v>22.289899999999999</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>-0.4</v>
       </c>
-      <c r="B44" s="28">
-        <v>8.1399500000000007</v>
+      <c r="B44" s="26">
+        <v>8.4659499999999994</v>
       </c>
       <c r="C44" s="25">
-        <v>22.289899999999999</v>
+        <v>20.210100000000001</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
-        <v>-0.4</v>
-      </c>
-      <c r="B45" s="26">
-        <v>8.4659499999999994</v>
+        <v>-0.8</v>
+      </c>
+      <c r="B45" s="29">
+        <v>1.5</v>
       </c>
       <c r="C45" s="25">
-        <v>20.210100000000001</v>
+        <v>64.978357503346302</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -27115,33 +27098,33 @@
         <v>-0.8</v>
       </c>
       <c r="B46" s="29">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="C46" s="25">
-        <v>64.978357503346302</v>
-      </c>
+        <v>61.187729099577801</v>
+      </c>
+      <c r="D46" s="27"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>-0.8</v>
       </c>
-      <c r="B47" s="29">
-        <v>2</v>
+      <c r="B47" s="28">
+        <v>2.5317099999999999</v>
       </c>
       <c r="C47" s="25">
-        <v>61.187729099577801</v>
-      </c>
-      <c r="D47" s="27"/>
+        <v>57.923000000000002</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>-0.8</v>
       </c>
       <c r="B48" s="28">
-        <v>2.5317099999999999</v>
+        <v>2.9331700000000001</v>
       </c>
       <c r="C48" s="25">
-        <v>57.923000000000002</v>
+        <v>54.055199999999999</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -27149,10 +27132,10 @@
         <v>-0.8</v>
       </c>
       <c r="B49" s="28">
-        <v>2.9331700000000001</v>
+        <v>3.3351199999999999</v>
       </c>
       <c r="C49" s="25">
-        <v>54.055199999999999</v>
+        <v>50.629399999999997</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -27160,10 +27143,10 @@
         <v>-0.8</v>
       </c>
       <c r="B50" s="28">
-        <v>3.3351199999999999</v>
+        <v>3.74865</v>
       </c>
       <c r="C50" s="25">
-        <v>50.629399999999997</v>
+        <v>47.771599999999999</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -27171,10 +27154,10 @@
         <v>-0.8</v>
       </c>
       <c r="B51" s="28">
-        <v>3.74865</v>
+        <v>4.1513600000000004</v>
       </c>
       <c r="C51" s="25">
-        <v>47.771599999999999</v>
+        <v>45.040599999999998</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -27182,10 +27165,10 @@
         <v>-0.8</v>
       </c>
       <c r="B52" s="28">
-        <v>4.1513600000000004</v>
+        <v>4.5542100000000003</v>
       </c>
       <c r="C52" s="25">
-        <v>45.040599999999998</v>
+        <v>42.4358</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -27193,32 +27176,32 @@
         <v>-0.8</v>
       </c>
       <c r="B53" s="28">
-        <v>4.5542100000000003</v>
+        <v>4.9573299999999998</v>
       </c>
       <c r="C53" s="25">
-        <v>42.4358</v>
+        <v>40.0837</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>-0.8</v>
       </c>
-      <c r="B54" s="28">
-        <v>4.9573299999999998</v>
+      <c r="B54" s="30">
+        <v>5.3608000000000002</v>
       </c>
       <c r="C54" s="25">
-        <v>40.0837</v>
+        <v>38.047400000000003</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>-0.8</v>
       </c>
-      <c r="B55" s="30">
-        <v>5.3608000000000002</v>
+      <c r="B55" s="28">
+        <v>5.7534400000000003</v>
       </c>
       <c r="C55" s="25">
-        <v>38.047400000000003</v>
+        <v>36.137799999999999</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -27226,10 +27209,10 @@
         <v>-0.8</v>
       </c>
       <c r="B56" s="28">
-        <v>5.7534400000000003</v>
+        <v>6.1569099999999999</v>
       </c>
       <c r="C56" s="25">
-        <v>36.137799999999999</v>
+        <v>34.101399999999998</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -27237,10 +27220,10 @@
         <v>-0.8</v>
       </c>
       <c r="B57" s="28">
-        <v>6.1569099999999999</v>
+        <v>6.5385200000000001</v>
       </c>
       <c r="C57" s="25">
-        <v>34.101399999999998</v>
+        <v>32.129100000000001</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -27248,10 +27231,10 @@
         <v>-0.8</v>
       </c>
       <c r="B58" s="28">
-        <v>6.5385200000000001</v>
+        <v>6.9530200000000004</v>
       </c>
       <c r="C58" s="25">
-        <v>32.129100000000001</v>
+        <v>30.1555</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -27259,10 +27242,10 @@
         <v>-0.8</v>
       </c>
       <c r="B59" s="28">
-        <v>6.9530200000000004</v>
+        <v>7.3454600000000001</v>
       </c>
       <c r="C59" s="25">
-        <v>30.1555</v>
+        <v>28.0564</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -27270,10 +27253,10 @@
         <v>-0.8</v>
       </c>
       <c r="B60" s="28">
-        <v>7.3454600000000001</v>
+        <v>7.7485799999999996</v>
       </c>
       <c r="C60" s="25">
-        <v>28.0564</v>
+        <v>25.7043</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -27281,10 +27264,10 @@
         <v>-0.8</v>
       </c>
       <c r="B61" s="28">
-        <v>7.7485799999999996</v>
+        <v>8.1516999999999999</v>
       </c>
       <c r="C61" s="25">
-        <v>25.7043</v>
+        <v>23.3521</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -27292,21 +27275,21 @@
         <v>-0.8</v>
       </c>
       <c r="B62" s="28">
-        <v>8.1516999999999999</v>
+        <v>8.4893099999999997</v>
       </c>
       <c r="C62" s="25">
-        <v>23.3521</v>
+        <v>21.255099999999999</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
-        <v>-0.8</v>
-      </c>
-      <c r="B63" s="28">
-        <v>8.4893099999999997</v>
+        <v>-1.6</v>
+      </c>
+      <c r="B63" s="29">
+        <v>1.5</v>
       </c>
       <c r="C63" s="25">
-        <v>21.255099999999999</v>
+        <v>66.837537792063102</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -27314,21 +27297,21 @@
         <v>-1.6</v>
       </c>
       <c r="B64" s="29">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="C64" s="25">
-        <v>66.837537792063102</v>
+        <v>63.4021616621988</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>-1.6</v>
       </c>
-      <c r="B65" s="29">
-        <v>2</v>
+      <c r="B65" s="30">
+        <v>2.53098</v>
       </c>
       <c r="C65" s="25">
-        <v>63.4021616621988</v>
+        <v>59.589700000000001</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -27336,10 +27319,10 @@
         <v>-1.6</v>
       </c>
       <c r="B66" s="30">
-        <v>2.53098</v>
+        <v>2.93221</v>
       </c>
       <c r="C66" s="25">
-        <v>59.589700000000001</v>
+        <v>56.716099999999997</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -27347,21 +27330,22 @@
         <v>-1.6</v>
       </c>
       <c r="B67" s="30">
-        <v>2.93221</v>
+        <v>3.33413</v>
       </c>
       <c r="C67" s="25">
-        <v>56.716099999999997</v>
-      </c>
+        <v>52.9223</v>
+      </c>
+      <c r="D67" s="27"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>-1.6</v>
       </c>
       <c r="B68" s="30">
-        <v>3.33413</v>
+        <v>3.7356799999999999</v>
       </c>
       <c r="C68" s="25">
-        <v>52.9223</v>
+        <v>49.619300000000003</v>
       </c>
       <c r="D68" s="27"/>
     </row>
@@ -27370,22 +27354,21 @@
         <v>-1.6</v>
       </c>
       <c r="B69" s="30">
-        <v>3.7356799999999999</v>
+        <v>4.1368299999999998</v>
       </c>
       <c r="C69" s="25">
-        <v>49.619300000000003</v>
-      </c>
-      <c r="D69" s="27"/>
+        <v>46.868400000000001</v>
+      </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>-1.6</v>
       </c>
       <c r="B70" s="30">
-        <v>4.1368299999999998</v>
+        <v>4.53789</v>
       </c>
       <c r="C70" s="25">
-        <v>46.868400000000001</v>
+        <v>44.240200000000002</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -27393,10 +27376,10 @@
         <v>-1.6</v>
       </c>
       <c r="B71" s="30">
-        <v>4.53789</v>
+        <v>4.9387600000000003</v>
       </c>
       <c r="C71" s="25">
-        <v>44.240200000000002</v>
+        <v>41.857399999999998</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -27404,10 +27387,10 @@
         <v>-1.6</v>
       </c>
       <c r="B72" s="30">
-        <v>4.9387600000000003</v>
+        <v>5.36172</v>
       </c>
       <c r="C72" s="25">
-        <v>41.857399999999998</v>
+        <v>39.597799999999999</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -27415,10 +27398,10 @@
         <v>-1.6</v>
       </c>
       <c r="B73" s="30">
-        <v>5.36172</v>
+        <v>5.7622299999999997</v>
       </c>
       <c r="C73" s="25">
-        <v>39.597799999999999</v>
+        <v>37.705800000000004</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -27426,10 +27409,10 @@
         <v>-1.6</v>
       </c>
       <c r="B74" s="30">
-        <v>5.7622299999999997</v>
+        <v>6.1627799999999997</v>
       </c>
       <c r="C74" s="25">
-        <v>37.705800000000004</v>
+        <v>35.752499999999998</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -27437,10 +27420,10 @@
         <v>-1.6</v>
       </c>
       <c r="B75" s="30">
-        <v>6.1627799999999997</v>
+        <v>6.5522099999999996</v>
       </c>
       <c r="C75" s="25">
-        <v>35.752499999999998</v>
+        <v>33.860199999999999</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -27448,10 +27431,10 @@
         <v>-1.6</v>
       </c>
       <c r="B76" s="30">
-        <v>6.5522099999999996</v>
+        <v>6.9527700000000001</v>
       </c>
       <c r="C76" s="25">
-        <v>33.860199999999999</v>
+        <v>31.9068</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -27459,10 +27442,10 @@
         <v>-1.6</v>
       </c>
       <c r="B77" s="30">
-        <v>6.9527700000000001</v>
+        <v>7.3644999999999996</v>
       </c>
       <c r="C77" s="25">
-        <v>31.9068</v>
+        <v>29.831</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -27470,10 +27453,10 @@
         <v>-1.6</v>
       </c>
       <c r="B78" s="30">
-        <v>7.3644999999999996</v>
+        <v>7.7542</v>
       </c>
       <c r="C78" s="25">
-        <v>29.831</v>
+        <v>27.570699999999999</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -27481,21 +27464,21 @@
         <v>-1.6</v>
       </c>
       <c r="B79" s="30">
-        <v>7.7542</v>
+        <v>8.4893400000000003</v>
       </c>
       <c r="C79" s="25">
-        <v>27.570699999999999</v>
+        <v>22.926100000000002</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
-        <v>-1.6</v>
-      </c>
-      <c r="B80" s="30">
-        <v>8.4893400000000003</v>
+        <v>-2</v>
+      </c>
+      <c r="B80" s="32">
+        <v>1.5</v>
       </c>
       <c r="C80" s="25">
-        <v>22.926100000000002</v>
+        <v>67.820060146011699</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -27503,10 +27486,10 @@
         <v>-2</v>
       </c>
       <c r="B81" s="32">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="C81" s="25">
-        <v>67.820060146011699</v>
+        <v>64.2361321255256</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -27514,10 +27497,10 @@
         <v>-2</v>
       </c>
       <c r="B82" s="32">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="C82" s="25">
-        <v>64.2361321255256</v>
+        <v>60.652204105039601</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -27525,10 +27508,10 @@
         <v>-2</v>
       </c>
       <c r="B83" s="32">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="C83" s="25">
-        <v>60.652204105039601</v>
+        <v>57.672656189740401</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -27536,10 +27519,10 @@
         <v>-2</v>
       </c>
       <c r="B84" s="32">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="C84" s="25">
-        <v>57.672656189740401</v>
+        <v>52.359609933403398</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -27547,10 +27530,10 @@
         <v>-2</v>
       </c>
       <c r="B85" s="32">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="C85" s="25">
-        <v>52.359609933403398</v>
+        <v>48.5559869999651</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -27558,10 +27541,10 @@
         <v>-2</v>
       </c>
       <c r="B86" s="32">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="C86" s="25">
-        <v>48.5559869999651</v>
+        <v>45.234724547231501</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -27569,10 +27552,10 @@
         <v>-2</v>
       </c>
       <c r="B87" s="32">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="C87" s="25">
-        <v>45.234724547231501</v>
+        <v>42.249216842405303</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -27580,10 +27563,10 @@
         <v>-2</v>
       </c>
       <c r="B88" s="32">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="C88" s="25">
-        <v>42.249216842405303</v>
+        <v>39.670879006627601</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -27591,10 +27574,10 @@
         <v>-2</v>
       </c>
       <c r="B89" s="32">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="C89" s="25">
-        <v>39.670879006627601</v>
+        <v>37.383330940208097</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -27602,10 +27585,10 @@
         <v>-2</v>
       </c>
       <c r="B90" s="32">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="C90" s="25">
-        <v>37.383330940208097</v>
+        <v>35.006692374260403</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -27613,10 +27596,10 @@
         <v>-2</v>
       </c>
       <c r="B91" s="32">
-        <v>6.5</v>
+        <v>7</v>
       </c>
       <c r="C91" s="25">
-        <v>35.006692374260403</v>
+        <v>32.595960869607502</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -27624,10 +27607,10 @@
         <v>-2</v>
       </c>
       <c r="B92" s="32">
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="C92" s="25">
-        <v>32.595960869607502</v>
+        <v>30.0943795017429</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -27635,10 +27618,10 @@
         <v>-2</v>
       </c>
       <c r="B93" s="32">
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="C93" s="25">
-        <v>30.0943795017429</v>
+        <v>26.960582876996298</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -27646,20 +27629,9 @@
         <v>-2</v>
       </c>
       <c r="B94" s="32">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="C94" s="25">
-        <v>26.960582876996298</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="4">
-        <v>-2</v>
-      </c>
-      <c r="B95" s="32">
-        <v>8.5</v>
-      </c>
-      <c r="C95" s="25">
         <v>23.701111515547598</v>
       </c>
     </row>

</xml_diff>

<commit_message>
sofia | bwl | fix
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/datasets/Stability/SSS_Sofia_Pantokarens_Angle_HydrostaticCurves.xlsx
+++ b/assets/fleet/9245263_sofia/datasets/Stability/SSS_Sofia_Pantokarens_Angle_HydrostaticCurves.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A7BD25F-E0FC-445C-B233-6AF3D2372785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C066F08-EB32-4857-B745-387C97AEAAF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Angle" sheetId="1" r:id="rId1"/>
@@ -1301,9 +1301,9 @@
   <sheetPr codeName="Лист2"/>
   <dimension ref="A1:Y218"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1468,7 +1468,7 @@
         <v>1</v>
       </c>
       <c r="T2" s="16">
-        <v>10.87</v>
+        <v>15.87</v>
       </c>
       <c r="U2" s="20" t="s">
         <v>1</v>
@@ -1543,7 +1543,7 @@
         <v>1</v>
       </c>
       <c r="T3" s="16">
-        <v>11.87</v>
+        <v>15.87</v>
       </c>
       <c r="U3" s="20" t="s">
         <v>1</v>
@@ -1618,7 +1618,7 @@
         <v>1</v>
       </c>
       <c r="T4" s="16">
-        <v>12.87</v>
+        <v>15.87</v>
       </c>
       <c r="U4" s="20" t="s">
         <v>1</v>
@@ -1693,7 +1693,7 @@
         <v>1</v>
       </c>
       <c r="T5" s="16">
-        <v>13.87</v>
+        <v>15.87</v>
       </c>
       <c r="U5" s="20" t="s">
         <v>1</v>
@@ -1768,7 +1768,7 @@
         <v>1</v>
       </c>
       <c r="T6" s="16">
-        <v>14.87</v>
+        <v>15.87</v>
       </c>
       <c r="U6" s="20" t="s">
         <v>1</v>
@@ -4168,7 +4168,7 @@
         <v>1</v>
       </c>
       <c r="T38" s="16">
-        <v>16.87</v>
+        <v>15.87</v>
       </c>
       <c r="U38" s="20" t="s">
         <v>1</v>
@@ -4243,7 +4243,7 @@
         <v>1</v>
       </c>
       <c r="T39" s="16">
-        <v>17.87</v>
+        <v>15.87</v>
       </c>
       <c r="U39" s="20" t="s">
         <v>1</v>
@@ -4318,7 +4318,7 @@
         <v>1</v>
       </c>
       <c r="T40" s="16">
-        <v>18.87</v>
+        <v>15.87</v>
       </c>
       <c r="U40" s="20" t="s">
         <v>1</v>
@@ -4393,7 +4393,7 @@
         <v>1</v>
       </c>
       <c r="T41" s="16">
-        <v>19.87</v>
+        <v>15.87</v>
       </c>
       <c r="U41" s="20" t="s">
         <v>1</v>
@@ -4468,7 +4468,7 @@
         <v>1</v>
       </c>
       <c r="T42" s="16">
-        <v>20.87</v>
+        <v>15.87</v>
       </c>
       <c r="U42" s="20" t="s">
         <v>1</v>
@@ -4544,7 +4544,7 @@
         <v>1</v>
       </c>
       <c r="T43" s="16">
-        <v>21.87</v>
+        <v>15.87</v>
       </c>
       <c r="U43" s="20" t="s">
         <v>1</v>
@@ -4619,7 +4619,7 @@
         <v>1</v>
       </c>
       <c r="T44" s="16">
-        <v>22.87</v>
+        <v>15.87</v>
       </c>
       <c r="U44" s="20" t="s">
         <v>1</v>
@@ -4694,7 +4694,7 @@
         <v>1</v>
       </c>
       <c r="T45" s="16">
-        <v>23.87</v>
+        <v>15.87</v>
       </c>
       <c r="U45" s="20" t="s">
         <v>1</v>
@@ -4769,7 +4769,7 @@
         <v>1</v>
       </c>
       <c r="T46" s="16">
-        <v>24.87</v>
+        <v>15.87</v>
       </c>
       <c r="U46" s="20" t="s">
         <v>1</v>
@@ -4844,7 +4844,7 @@
         <v>1</v>
       </c>
       <c r="T47" s="16">
-        <v>25.87</v>
+        <v>15.87</v>
       </c>
       <c r="U47" s="20" t="s">
         <v>1</v>
@@ -4919,7 +4919,7 @@
         <v>1</v>
       </c>
       <c r="T48" s="16">
-        <v>26.87</v>
+        <v>15.87</v>
       </c>
       <c r="U48" s="20" t="s">
         <v>1</v>
@@ -4994,7 +4994,7 @@
         <v>1</v>
       </c>
       <c r="T49" s="16">
-        <v>27.87</v>
+        <v>15.87</v>
       </c>
       <c r="U49" s="20" t="s">
         <v>1</v>
@@ -5069,7 +5069,7 @@
         <v>1</v>
       </c>
       <c r="T50" s="16">
-        <v>28.87</v>
+        <v>15.87</v>
       </c>
       <c r="U50" s="20" t="s">
         <v>1</v>
@@ -5144,7 +5144,7 @@
         <v>1</v>
       </c>
       <c r="T51" s="16">
-        <v>29.87</v>
+        <v>15.87</v>
       </c>
       <c r="U51" s="20" t="s">
         <v>1</v>
@@ -5219,7 +5219,7 @@
         <v>1</v>
       </c>
       <c r="T52" s="16">
-        <v>30.87</v>
+        <v>15.87</v>
       </c>
       <c r="U52" s="20" t="s">
         <v>1</v>
@@ -5294,7 +5294,7 @@
         <v>1</v>
       </c>
       <c r="T53" s="16">
-        <v>31.87</v>
+        <v>15.87</v>
       </c>
       <c r="U53" s="20" t="s">
         <v>1</v>
@@ -5369,7 +5369,7 @@
         <v>1</v>
       </c>
       <c r="T54" s="16">
-        <v>32.869999999999997</v>
+        <v>15.87</v>
       </c>
       <c r="U54" s="20" t="s">
         <v>1</v>
@@ -5444,7 +5444,7 @@
         <v>1</v>
       </c>
       <c r="T55" s="16">
-        <v>33.869999999999997</v>
+        <v>15.87</v>
       </c>
       <c r="U55" s="20" t="s">
         <v>1</v>
@@ -5519,7 +5519,7 @@
         <v>1</v>
       </c>
       <c r="T56" s="16">
-        <v>34.869999999999997</v>
+        <v>15.87</v>
       </c>
       <c r="U56" s="20" t="s">
         <v>1</v>
@@ -5594,7 +5594,7 @@
         <v>1</v>
       </c>
       <c r="T57" s="16">
-        <v>35.869999999999997</v>
+        <v>15.87</v>
       </c>
       <c r="U57" s="20" t="s">
         <v>1</v>
@@ -5669,7 +5669,7 @@
         <v>1</v>
       </c>
       <c r="T58" s="16">
-        <v>36.869999999999997</v>
+        <v>15.87</v>
       </c>
       <c r="U58" s="20" t="s">
         <v>1</v>
@@ -5744,7 +5744,7 @@
         <v>1</v>
       </c>
       <c r="T59" s="16">
-        <v>37.869999999999997</v>
+        <v>15.87</v>
       </c>
       <c r="U59" s="20" t="s">
         <v>1</v>
@@ -5819,7 +5819,7 @@
         <v>1</v>
       </c>
       <c r="T60" s="16">
-        <v>38.869999999999997</v>
+        <v>15.87</v>
       </c>
       <c r="U60" s="20" t="s">
         <v>1</v>
@@ -5894,7 +5894,7 @@
         <v>1</v>
       </c>
       <c r="T61" s="16">
-        <v>39.869999999999997</v>
+        <v>15.87</v>
       </c>
       <c r="U61" s="20" t="s">
         <v>1</v>
@@ -5969,7 +5969,7 @@
         <v>1</v>
       </c>
       <c r="T62" s="16">
-        <v>40.869999999999997</v>
+        <v>15.87</v>
       </c>
       <c r="U62" s="20" t="s">
         <v>1</v>
@@ -6044,7 +6044,7 @@
         <v>1</v>
       </c>
       <c r="T63" s="16">
-        <v>41.87</v>
+        <v>15.87</v>
       </c>
       <c r="U63" s="20" t="s">
         <v>1</v>
@@ -6119,7 +6119,7 @@
         <v>1</v>
       </c>
       <c r="T64" s="16">
-        <v>42.87</v>
+        <v>15.87</v>
       </c>
       <c r="U64" s="20" t="s">
         <v>1</v>
@@ -6194,7 +6194,7 @@
         <v>1</v>
       </c>
       <c r="T65" s="16">
-        <v>43.87</v>
+        <v>15.87</v>
       </c>
       <c r="U65" s="20" t="s">
         <v>1</v>
@@ -6269,7 +6269,7 @@
         <v>1</v>
       </c>
       <c r="T66" s="16">
-        <v>44.87</v>
+        <v>15.87</v>
       </c>
       <c r="U66" s="20" t="s">
         <v>1</v>
@@ -6344,7 +6344,7 @@
         <v>1</v>
       </c>
       <c r="T67" s="16">
-        <v>45.87</v>
+        <v>15.87</v>
       </c>
       <c r="U67" s="20" t="s">
         <v>1</v>
@@ -6419,7 +6419,7 @@
         <v>1</v>
       </c>
       <c r="T68" s="16">
-        <v>46.87</v>
+        <v>15.87</v>
       </c>
       <c r="U68" s="20" t="s">
         <v>1</v>
@@ -6494,7 +6494,7 @@
         <v>1</v>
       </c>
       <c r="T69" s="16">
-        <v>47.87</v>
+        <v>15.87</v>
       </c>
       <c r="U69" s="20" t="s">
         <v>1</v>
@@ -6569,7 +6569,7 @@
         <v>1</v>
       </c>
       <c r="T70" s="16">
-        <v>48.87</v>
+        <v>15.87</v>
       </c>
       <c r="U70" s="20" t="s">
         <v>1</v>
@@ -6644,7 +6644,7 @@
         <v>1</v>
       </c>
       <c r="T71" s="16">
-        <v>49.87</v>
+        <v>15.87</v>
       </c>
       <c r="U71" s="20" t="s">
         <v>1</v>
@@ -6719,7 +6719,7 @@
         <v>1</v>
       </c>
       <c r="T72" s="16">
-        <v>50.87</v>
+        <v>15.87</v>
       </c>
       <c r="U72" s="20" t="s">
         <v>1</v>
@@ -6794,7 +6794,7 @@
         <v>1</v>
       </c>
       <c r="T73" s="16">
-        <v>51.87</v>
+        <v>15.87</v>
       </c>
       <c r="U73" s="20" t="s">
         <v>1</v>
@@ -6868,7 +6868,7 @@
         <v>1</v>
       </c>
       <c r="T74" s="16">
-        <v>52.87</v>
+        <v>15.87</v>
       </c>
       <c r="U74" s="20" t="s">
         <v>1</v>
@@ -6943,7 +6943,7 @@
         <v>1</v>
       </c>
       <c r="T75" s="16">
-        <v>53.87</v>
+        <v>15.87</v>
       </c>
       <c r="U75" s="20" t="s">
         <v>1</v>
@@ -7018,7 +7018,7 @@
         <v>1</v>
       </c>
       <c r="T76" s="16">
-        <v>54.87</v>
+        <v>15.87</v>
       </c>
       <c r="U76" s="20" t="s">
         <v>1</v>
@@ -7093,7 +7093,7 @@
         <v>1</v>
       </c>
       <c r="T77" s="16">
-        <v>55.87</v>
+        <v>15.87</v>
       </c>
       <c r="U77" s="20" t="s">
         <v>1</v>
@@ -7168,7 +7168,7 @@
         <v>1</v>
       </c>
       <c r="T78" s="16">
-        <v>56.87</v>
+        <v>15.87</v>
       </c>
       <c r="U78" s="20" t="s">
         <v>1</v>
@@ -7244,7 +7244,7 @@
         <v>1</v>
       </c>
       <c r="T79" s="16">
-        <v>57.87</v>
+        <v>15.87</v>
       </c>
       <c r="U79" s="20" t="s">
         <v>1</v>
@@ -7319,7 +7319,7 @@
         <v>1</v>
       </c>
       <c r="T80" s="16">
-        <v>58.87</v>
+        <v>15.87</v>
       </c>
       <c r="U80" s="20" t="s">
         <v>1</v>
@@ -7394,7 +7394,7 @@
         <v>1</v>
       </c>
       <c r="T81" s="16">
-        <v>59.87</v>
+        <v>15.87</v>
       </c>
       <c r="U81" s="20" t="s">
         <v>1</v>
@@ -7469,7 +7469,7 @@
         <v>1</v>
       </c>
       <c r="T82" s="16">
-        <v>60.87</v>
+        <v>15.87</v>
       </c>
       <c r="U82" s="20" t="s">
         <v>1</v>
@@ -7544,7 +7544,7 @@
         <v>1</v>
       </c>
       <c r="T83" s="16">
-        <v>61.87</v>
+        <v>15.87</v>
       </c>
       <c r="U83" s="20" t="s">
         <v>1</v>
@@ -7619,7 +7619,7 @@
         <v>1</v>
       </c>
       <c r="T84" s="16">
-        <v>62.87</v>
+        <v>15.87</v>
       </c>
       <c r="U84" s="20" t="s">
         <v>1</v>
@@ -7694,7 +7694,7 @@
         <v>1</v>
       </c>
       <c r="T85" s="16">
-        <v>63.87</v>
+        <v>15.87</v>
       </c>
       <c r="U85" s="20" t="s">
         <v>1</v>
@@ -7769,7 +7769,7 @@
         <v>1</v>
       </c>
       <c r="T86" s="16">
-        <v>64.87</v>
+        <v>15.87</v>
       </c>
       <c r="U86" s="20" t="s">
         <v>1</v>
@@ -7844,7 +7844,7 @@
         <v>1</v>
       </c>
       <c r="T87" s="16">
-        <v>65.87</v>
+        <v>15.87</v>
       </c>
       <c r="U87" s="20" t="s">
         <v>1</v>
@@ -7919,7 +7919,7 @@
         <v>1</v>
       </c>
       <c r="T88" s="16">
-        <v>66.87</v>
+        <v>15.87</v>
       </c>
       <c r="U88" s="20" t="s">
         <v>1</v>
@@ -7994,7 +7994,7 @@
         <v>1</v>
       </c>
       <c r="T89" s="16">
-        <v>67.87</v>
+        <v>15.87</v>
       </c>
       <c r="U89" s="20" t="s">
         <v>1</v>
@@ -8069,7 +8069,7 @@
         <v>1</v>
       </c>
       <c r="T90" s="16">
-        <v>68.87</v>
+        <v>15.87</v>
       </c>
       <c r="U90" s="20" t="s">
         <v>1</v>
@@ -8144,7 +8144,7 @@
         <v>1</v>
       </c>
       <c r="T91" s="16">
-        <v>69.87</v>
+        <v>15.87</v>
       </c>
       <c r="U91" s="20" t="s">
         <v>1</v>
@@ -8219,7 +8219,7 @@
         <v>1</v>
       </c>
       <c r="T92" s="16">
-        <v>70.87</v>
+        <v>15.87</v>
       </c>
       <c r="U92" s="20" t="s">
         <v>1</v>
@@ -8294,7 +8294,7 @@
         <v>1</v>
       </c>
       <c r="T93" s="16">
-        <v>71.87</v>
+        <v>15.87</v>
       </c>
       <c r="U93" s="20" t="s">
         <v>1</v>
@@ -8369,7 +8369,7 @@
         <v>1</v>
       </c>
       <c r="T94" s="16">
-        <v>72.87</v>
+        <v>15.87</v>
       </c>
       <c r="U94" s="20" t="s">
         <v>1</v>
@@ -8444,7 +8444,7 @@
         <v>1</v>
       </c>
       <c r="T95" s="16">
-        <v>73.87</v>
+        <v>15.87</v>
       </c>
       <c r="U95" s="20" t="s">
         <v>1</v>
@@ -8519,7 +8519,7 @@
         <v>1</v>
       </c>
       <c r="T96" s="16">
-        <v>74.87</v>
+        <v>15.87</v>
       </c>
       <c r="U96" s="20" t="s">
         <v>1</v>
@@ -8594,7 +8594,7 @@
         <v>1</v>
       </c>
       <c r="T97" s="16">
-        <v>75.87</v>
+        <v>15.87</v>
       </c>
       <c r="U97" s="20" t="s">
         <v>1</v>
@@ -8669,7 +8669,7 @@
         <v>1</v>
       </c>
       <c r="T98" s="16">
-        <v>76.87</v>
+        <v>15.87</v>
       </c>
       <c r="U98" s="20" t="s">
         <v>1</v>
@@ -8744,7 +8744,7 @@
         <v>1</v>
       </c>
       <c r="T99" s="16">
-        <v>77.87</v>
+        <v>15.87</v>
       </c>
       <c r="U99" s="20" t="s">
         <v>1</v>
@@ -8819,7 +8819,7 @@
         <v>1</v>
       </c>
       <c r="T100" s="16">
-        <v>78.87</v>
+        <v>15.87</v>
       </c>
       <c r="U100" s="20" t="s">
         <v>1</v>
@@ -8894,7 +8894,7 @@
         <v>1</v>
       </c>
       <c r="T101" s="16">
-        <v>79.87</v>
+        <v>15.87</v>
       </c>
       <c r="U101" s="20" t="s">
         <v>1</v>
@@ -8969,7 +8969,7 @@
         <v>1</v>
       </c>
       <c r="T102" s="16">
-        <v>80.87</v>
+        <v>15.87</v>
       </c>
       <c r="U102" s="20" t="s">
         <v>1</v>
@@ -9044,7 +9044,7 @@
         <v>1</v>
       </c>
       <c r="T103" s="16">
-        <v>81.87</v>
+        <v>15.87</v>
       </c>
       <c r="U103" s="20" t="s">
         <v>1</v>
@@ -9119,7 +9119,7 @@
         <v>1</v>
       </c>
       <c r="T104" s="16">
-        <v>82.87</v>
+        <v>15.87</v>
       </c>
       <c r="U104" s="20" t="s">
         <v>1</v>
@@ -9194,7 +9194,7 @@
         <v>1</v>
       </c>
       <c r="T105" s="16">
-        <v>83.87</v>
+        <v>15.87</v>
       </c>
       <c r="U105" s="20" t="s">
         <v>1</v>
@@ -9269,7 +9269,7 @@
         <v>1</v>
       </c>
       <c r="T106" s="16">
-        <v>84.87</v>
+        <v>15.87</v>
       </c>
       <c r="U106" s="20" t="s">
         <v>1</v>
@@ -9344,7 +9344,7 @@
         <v>1</v>
       </c>
       <c r="T107" s="16">
-        <v>85.87</v>
+        <v>15.87</v>
       </c>
       <c r="U107" s="20" t="s">
         <v>1</v>
@@ -9419,7 +9419,7 @@
         <v>1</v>
       </c>
       <c r="T108" s="16">
-        <v>86.87</v>
+        <v>15.87</v>
       </c>
       <c r="U108" s="20" t="s">
         <v>1</v>
@@ -9494,7 +9494,7 @@
         <v>1</v>
       </c>
       <c r="T109" s="16">
-        <v>87.87</v>
+        <v>15.87</v>
       </c>
       <c r="U109" s="20" t="s">
         <v>1</v>
@@ -9568,7 +9568,7 @@
         <v>1</v>
       </c>
       <c r="T110" s="16">
-        <v>88.87</v>
+        <v>15.87</v>
       </c>
       <c r="U110" s="20" t="s">
         <v>1</v>
@@ -9644,7 +9644,7 @@
         <v>1</v>
       </c>
       <c r="T111" s="16">
-        <v>89.87</v>
+        <v>15.87</v>
       </c>
       <c r="U111" s="20" t="s">
         <v>1</v>
@@ -9720,7 +9720,7 @@
         <v>1</v>
       </c>
       <c r="T112" s="16">
-        <v>90.87</v>
+        <v>15.87</v>
       </c>
       <c r="U112" s="20" t="s">
         <v>1</v>
@@ -9796,7 +9796,7 @@
         <v>1</v>
       </c>
       <c r="T113" s="16">
-        <v>91.87</v>
+        <v>15.87</v>
       </c>
       <c r="U113" s="20" t="s">
         <v>1</v>
@@ -9872,7 +9872,7 @@
         <v>1</v>
       </c>
       <c r="T114" s="16">
-        <v>92.87</v>
+        <v>15.87</v>
       </c>
       <c r="U114" s="20" t="s">
         <v>1</v>
@@ -9949,7 +9949,7 @@
         <v>1</v>
       </c>
       <c r="T115" s="16">
-        <v>93.87</v>
+        <v>15.87</v>
       </c>
       <c r="U115" s="20" t="s">
         <v>1</v>
@@ -10025,7 +10025,7 @@
         <v>1</v>
       </c>
       <c r="T116" s="16">
-        <v>94.87</v>
+        <v>15.87</v>
       </c>
       <c r="U116" s="20" t="s">
         <v>1</v>
@@ -10100,7 +10100,7 @@
         <v>1</v>
       </c>
       <c r="T117" s="16">
-        <v>95.87</v>
+        <v>15.87</v>
       </c>
       <c r="U117" s="20" t="s">
         <v>1</v>
@@ -10175,7 +10175,7 @@
         <v>1</v>
       </c>
       <c r="T118" s="16">
-        <v>96.87</v>
+        <v>15.87</v>
       </c>
       <c r="U118" s="20" t="s">
         <v>1</v>
@@ -10250,7 +10250,7 @@
         <v>1</v>
       </c>
       <c r="T119" s="16">
-        <v>97.87</v>
+        <v>15.87</v>
       </c>
       <c r="U119" s="20" t="s">
         <v>1</v>
@@ -10325,7 +10325,7 @@
         <v>1</v>
       </c>
       <c r="T120" s="16">
-        <v>98.87</v>
+        <v>15.87</v>
       </c>
       <c r="U120" s="20" t="s">
         <v>1</v>
@@ -10400,7 +10400,7 @@
         <v>1</v>
       </c>
       <c r="T121" s="16">
-        <v>99.87</v>
+        <v>15.87</v>
       </c>
       <c r="U121" s="20" t="s">
         <v>1</v>
@@ -10475,7 +10475,7 @@
         <v>1</v>
       </c>
       <c r="T122" s="16">
-        <v>100.87</v>
+        <v>15.87</v>
       </c>
       <c r="U122" s="20" t="s">
         <v>1</v>
@@ -10550,7 +10550,7 @@
         <v>1</v>
       </c>
       <c r="T123" s="16">
-        <v>101.87</v>
+        <v>15.87</v>
       </c>
       <c r="U123" s="20" t="s">
         <v>1</v>
@@ -10625,7 +10625,7 @@
         <v>1</v>
       </c>
       <c r="T124" s="16">
-        <v>102.87</v>
+        <v>15.87</v>
       </c>
       <c r="U124" s="20" t="s">
         <v>1</v>
@@ -10700,7 +10700,7 @@
         <v>1</v>
       </c>
       <c r="T125" s="16">
-        <v>103.87</v>
+        <v>15.87</v>
       </c>
       <c r="U125" s="20" t="s">
         <v>1</v>
@@ -10775,7 +10775,7 @@
         <v>1</v>
       </c>
       <c r="T126" s="16">
-        <v>104.87</v>
+        <v>15.87</v>
       </c>
       <c r="U126" s="20" t="s">
         <v>1</v>
@@ -10850,7 +10850,7 @@
         <v>1</v>
       </c>
       <c r="T127" s="16">
-        <v>105.87</v>
+        <v>15.87</v>
       </c>
       <c r="U127" s="20" t="s">
         <v>1</v>
@@ -10925,7 +10925,7 @@
         <v>1</v>
       </c>
       <c r="T128" s="16">
-        <v>106.87</v>
+        <v>15.87</v>
       </c>
       <c r="U128" s="20" t="s">
         <v>1</v>
@@ -11000,7 +11000,7 @@
         <v>1</v>
       </c>
       <c r="T129" s="16">
-        <v>107.87</v>
+        <v>15.87</v>
       </c>
       <c r="U129" s="20" t="s">
         <v>1</v>
@@ -11075,7 +11075,7 @@
         <v>1</v>
       </c>
       <c r="T130" s="16">
-        <v>108.87</v>
+        <v>15.87</v>
       </c>
       <c r="U130" s="20" t="s">
         <v>1</v>
@@ -11150,7 +11150,7 @@
         <v>1</v>
       </c>
       <c r="T131" s="16">
-        <v>109.87</v>
+        <v>15.87</v>
       </c>
       <c r="U131" s="20" t="s">
         <v>1</v>
@@ -11225,7 +11225,7 @@
         <v>1</v>
       </c>
       <c r="T132" s="16">
-        <v>110.87</v>
+        <v>15.87</v>
       </c>
       <c r="U132" s="20" t="s">
         <v>1</v>
@@ -11300,7 +11300,7 @@
         <v>1</v>
       </c>
       <c r="T133" s="16">
-        <v>111.87</v>
+        <v>15.87</v>
       </c>
       <c r="U133" s="20" t="s">
         <v>1</v>
@@ -11375,7 +11375,7 @@
         <v>1</v>
       </c>
       <c r="T134" s="16">
-        <v>112.87</v>
+        <v>15.87</v>
       </c>
       <c r="U134" s="20" t="s">
         <v>1</v>
@@ -11450,7 +11450,7 @@
         <v>1</v>
       </c>
       <c r="T135" s="16">
-        <v>113.87</v>
+        <v>15.87</v>
       </c>
       <c r="U135" s="20" t="s">
         <v>1</v>
@@ -11525,7 +11525,7 @@
         <v>1</v>
       </c>
       <c r="T136" s="16">
-        <v>114.87</v>
+        <v>15.87</v>
       </c>
       <c r="U136" s="20" t="s">
         <v>1</v>
@@ -11600,7 +11600,7 @@
         <v>1</v>
       </c>
       <c r="T137" s="16">
-        <v>115.87</v>
+        <v>15.87</v>
       </c>
       <c r="U137" s="20" t="s">
         <v>1</v>
@@ -11675,7 +11675,7 @@
         <v>1</v>
       </c>
       <c r="T138" s="16">
-        <v>116.87</v>
+        <v>15.87</v>
       </c>
       <c r="U138" s="20" t="s">
         <v>1</v>
@@ -11750,7 +11750,7 @@
         <v>1</v>
       </c>
       <c r="T139" s="16">
-        <v>117.87</v>
+        <v>15.87</v>
       </c>
       <c r="U139" s="20" t="s">
         <v>1</v>
@@ -11825,7 +11825,7 @@
         <v>1</v>
       </c>
       <c r="T140" s="16">
-        <v>118.87</v>
+        <v>15.87</v>
       </c>
       <c r="U140" s="20" t="s">
         <v>1</v>
@@ -11900,7 +11900,7 @@
         <v>1</v>
       </c>
       <c r="T141" s="16">
-        <v>119.87</v>
+        <v>15.87</v>
       </c>
       <c r="U141" s="20" t="s">
         <v>1</v>
@@ -11975,7 +11975,7 @@
         <v>1</v>
       </c>
       <c r="T142" s="16">
-        <v>120.87</v>
+        <v>15.87</v>
       </c>
       <c r="U142" s="20" t="s">
         <v>1</v>
@@ -12050,7 +12050,7 @@
         <v>1</v>
       </c>
       <c r="T143" s="16">
-        <v>121.87</v>
+        <v>15.87</v>
       </c>
       <c r="U143" s="20" t="s">
         <v>1</v>
@@ -12125,7 +12125,7 @@
         <v>1</v>
       </c>
       <c r="T144" s="16">
-        <v>122.87</v>
+        <v>15.87</v>
       </c>
       <c r="U144" s="20" t="s">
         <v>1</v>
@@ -12200,7 +12200,7 @@
         <v>1</v>
       </c>
       <c r="T145" s="16">
-        <v>123.87</v>
+        <v>15.87</v>
       </c>
       <c r="U145" s="20" t="s">
         <v>1</v>
@@ -12274,7 +12274,7 @@
         <v>1</v>
       </c>
       <c r="T146" s="16">
-        <v>124.87</v>
+        <v>15.87</v>
       </c>
       <c r="U146" s="20" t="s">
         <v>1</v>
@@ -12349,7 +12349,7 @@
         <v>1</v>
       </c>
       <c r="T147" s="16">
-        <v>125.87</v>
+        <v>15.87</v>
       </c>
       <c r="U147" s="20" t="s">
         <v>1</v>
@@ -12424,7 +12424,7 @@
         <v>1</v>
       </c>
       <c r="T148" s="16">
-        <v>126.87</v>
+        <v>15.87</v>
       </c>
       <c r="U148" s="20" t="s">
         <v>1</v>
@@ -12499,7 +12499,7 @@
         <v>1</v>
       </c>
       <c r="T149" s="16">
-        <v>127.87</v>
+        <v>15.87</v>
       </c>
       <c r="U149" s="20" t="s">
         <v>1</v>
@@ -12574,7 +12574,7 @@
         <v>1</v>
       </c>
       <c r="T150" s="16">
-        <v>128.87</v>
+        <v>15.87</v>
       </c>
       <c r="U150" s="20" t="s">
         <v>1</v>
@@ -12650,7 +12650,7 @@
         <v>1</v>
       </c>
       <c r="T151" s="16">
-        <v>129.87</v>
+        <v>15.87</v>
       </c>
       <c r="U151" s="20" t="s">
         <v>1</v>
@@ -12725,7 +12725,7 @@
         <v>1</v>
       </c>
       <c r="T152" s="16">
-        <v>130.87</v>
+        <v>15.87</v>
       </c>
       <c r="U152" s="20" t="s">
         <v>1</v>
@@ -12800,7 +12800,7 @@
         <v>1</v>
       </c>
       <c r="T153" s="16">
-        <v>131.87</v>
+        <v>15.87</v>
       </c>
       <c r="U153" s="20" t="s">
         <v>1</v>
@@ -12875,7 +12875,7 @@
         <v>1</v>
       </c>
       <c r="T154" s="16">
-        <v>132.87</v>
+        <v>15.87</v>
       </c>
       <c r="U154" s="20" t="s">
         <v>1</v>
@@ -12950,7 +12950,7 @@
         <v>1</v>
       </c>
       <c r="T155" s="16">
-        <v>133.87</v>
+        <v>15.87</v>
       </c>
       <c r="U155" s="20" t="s">
         <v>1</v>
@@ -13025,7 +13025,7 @@
         <v>1</v>
       </c>
       <c r="T156" s="16">
-        <v>134.87</v>
+        <v>15.87</v>
       </c>
       <c r="U156" s="20" t="s">
         <v>1</v>
@@ -13100,7 +13100,7 @@
         <v>1</v>
       </c>
       <c r="T157" s="16">
-        <v>135.87</v>
+        <v>15.87</v>
       </c>
       <c r="U157" s="20" t="s">
         <v>1</v>
@@ -13175,7 +13175,7 @@
         <v>1</v>
       </c>
       <c r="T158" s="16">
-        <v>136.87</v>
+        <v>15.87</v>
       </c>
       <c r="U158" s="20" t="s">
         <v>1</v>
@@ -13250,7 +13250,7 @@
         <v>1</v>
       </c>
       <c r="T159" s="16">
-        <v>137.87</v>
+        <v>15.87</v>
       </c>
       <c r="U159" s="20" t="s">
         <v>1</v>
@@ -13325,7 +13325,7 @@
         <v>1</v>
       </c>
       <c r="T160" s="16">
-        <v>138.87</v>
+        <v>15.87</v>
       </c>
       <c r="U160" s="20" t="s">
         <v>1</v>
@@ -13400,7 +13400,7 @@
         <v>1</v>
       </c>
       <c r="T161" s="16">
-        <v>139.87</v>
+        <v>15.87</v>
       </c>
       <c r="U161" s="20" t="s">
         <v>1</v>
@@ -13475,7 +13475,7 @@
         <v>1</v>
       </c>
       <c r="T162" s="16">
-        <v>140.87</v>
+        <v>15.87</v>
       </c>
       <c r="U162" s="20" t="s">
         <v>1</v>
@@ -13550,7 +13550,7 @@
         <v>1</v>
       </c>
       <c r="T163" s="16">
-        <v>141.87</v>
+        <v>15.87</v>
       </c>
       <c r="U163" s="20" t="s">
         <v>1</v>
@@ -13625,7 +13625,7 @@
         <v>1</v>
       </c>
       <c r="T164" s="16">
-        <v>142.87</v>
+        <v>15.87</v>
       </c>
       <c r="U164" s="20" t="s">
         <v>1</v>
@@ -13700,7 +13700,7 @@
         <v>1</v>
       </c>
       <c r="T165" s="16">
-        <v>143.87</v>
+        <v>15.87</v>
       </c>
       <c r="U165" s="20" t="s">
         <v>1</v>
@@ -13775,7 +13775,7 @@
         <v>1</v>
       </c>
       <c r="T166" s="16">
-        <v>144.87</v>
+        <v>15.87</v>
       </c>
       <c r="U166" s="20" t="s">
         <v>1</v>
@@ -13850,7 +13850,7 @@
         <v>1</v>
       </c>
       <c r="T167" s="16">
-        <v>145.87</v>
+        <v>15.87</v>
       </c>
       <c r="U167" s="20" t="s">
         <v>1</v>
@@ -13925,7 +13925,7 @@
         <v>1</v>
       </c>
       <c r="T168" s="16">
-        <v>146.87</v>
+        <v>15.87</v>
       </c>
       <c r="U168" s="20" t="s">
         <v>1</v>
@@ -14000,7 +14000,7 @@
         <v>1</v>
       </c>
       <c r="T169" s="16">
-        <v>147.87</v>
+        <v>15.87</v>
       </c>
       <c r="U169" s="20" t="s">
         <v>1</v>
@@ -14075,7 +14075,7 @@
         <v>1</v>
       </c>
       <c r="T170" s="16">
-        <v>148.87</v>
+        <v>15.87</v>
       </c>
       <c r="U170" s="20" t="s">
         <v>1</v>
@@ -14150,7 +14150,7 @@
         <v>1</v>
       </c>
       <c r="T171" s="16">
-        <v>149.87</v>
+        <v>15.87</v>
       </c>
       <c r="U171" s="20" t="s">
         <v>1</v>
@@ -14225,7 +14225,7 @@
         <v>1</v>
       </c>
       <c r="T172" s="16">
-        <v>150.87</v>
+        <v>15.87</v>
       </c>
       <c r="U172" s="20" t="s">
         <v>1</v>
@@ -14300,7 +14300,7 @@
         <v>1</v>
       </c>
       <c r="T173" s="16">
-        <v>151.87</v>
+        <v>15.87</v>
       </c>
       <c r="U173" s="20" t="s">
         <v>1</v>
@@ -14375,7 +14375,7 @@
         <v>1</v>
       </c>
       <c r="T174" s="16">
-        <v>152.87</v>
+        <v>15.87</v>
       </c>
       <c r="U174" s="20" t="s">
         <v>1</v>
@@ -14450,7 +14450,7 @@
         <v>1</v>
       </c>
       <c r="T175" s="16">
-        <v>153.87</v>
+        <v>15.87</v>
       </c>
       <c r="U175" s="20" t="s">
         <v>1</v>
@@ -14525,7 +14525,7 @@
         <v>1</v>
       </c>
       <c r="T176" s="16">
-        <v>154.87</v>
+        <v>15.87</v>
       </c>
       <c r="U176" s="20" t="s">
         <v>1</v>
@@ -14600,7 +14600,7 @@
         <v>1</v>
       </c>
       <c r="T177" s="16">
-        <v>155.87</v>
+        <v>15.87</v>
       </c>
       <c r="U177" s="20" t="s">
         <v>1</v>
@@ -14675,7 +14675,7 @@
         <v>1</v>
       </c>
       <c r="T178" s="16">
-        <v>156.87</v>
+        <v>15.87</v>
       </c>
       <c r="U178" s="20" t="s">
         <v>1</v>
@@ -14750,7 +14750,7 @@
         <v>1</v>
       </c>
       <c r="T179" s="16">
-        <v>157.87</v>
+        <v>15.87</v>
       </c>
       <c r="U179" s="20" t="s">
         <v>1</v>
@@ -14825,7 +14825,7 @@
         <v>1</v>
       </c>
       <c r="T180" s="16">
-        <v>158.87</v>
+        <v>15.87</v>
       </c>
       <c r="U180" s="20" t="s">
         <v>1</v>
@@ -14900,7 +14900,7 @@
         <v>1</v>
       </c>
       <c r="T181" s="16">
-        <v>159.87</v>
+        <v>15.87</v>
       </c>
       <c r="U181" s="20" t="s">
         <v>1</v>
@@ -14974,7 +14974,7 @@
         <v>1</v>
       </c>
       <c r="T182" s="16">
-        <v>160.87</v>
+        <v>15.87</v>
       </c>
       <c r="U182" s="20" t="s">
         <v>1</v>
@@ -15049,7 +15049,7 @@
         <v>1</v>
       </c>
       <c r="T183" s="16">
-        <v>161.87</v>
+        <v>15.87</v>
       </c>
       <c r="U183" s="20" t="s">
         <v>1</v>
@@ -15124,7 +15124,7 @@
         <v>1</v>
       </c>
       <c r="T184" s="16">
-        <v>162.87</v>
+        <v>15.87</v>
       </c>
       <c r="U184" s="20" t="s">
         <v>1</v>
@@ -15199,7 +15199,7 @@
         <v>1</v>
       </c>
       <c r="T185" s="16">
-        <v>163.87</v>
+        <v>15.87</v>
       </c>
       <c r="U185" s="20" t="s">
         <v>1</v>
@@ -15274,7 +15274,7 @@
         <v>1</v>
       </c>
       <c r="T186" s="16">
-        <v>164.87</v>
+        <v>15.87</v>
       </c>
       <c r="U186" s="20" t="s">
         <v>1</v>
@@ -15350,7 +15350,7 @@
         <v>1</v>
       </c>
       <c r="T187" s="16">
-        <v>165.87</v>
+        <v>15.87</v>
       </c>
       <c r="U187" s="20" t="s">
         <v>1</v>
@@ -15425,7 +15425,7 @@
         <v>1</v>
       </c>
       <c r="T188" s="16">
-        <v>166.87</v>
+        <v>15.87</v>
       </c>
       <c r="U188" s="20" t="s">
         <v>1</v>
@@ -15500,7 +15500,7 @@
         <v>1</v>
       </c>
       <c r="T189" s="16">
-        <v>167.87</v>
+        <v>15.87</v>
       </c>
       <c r="U189" s="20" t="s">
         <v>1</v>
@@ -15575,7 +15575,7 @@
         <v>1</v>
       </c>
       <c r="T190" s="16">
-        <v>168.87</v>
+        <v>15.87</v>
       </c>
       <c r="U190" s="20" t="s">
         <v>1</v>
@@ -15650,7 +15650,7 @@
         <v>1</v>
       </c>
       <c r="T191" s="16">
-        <v>169.87</v>
+        <v>15.87</v>
       </c>
       <c r="U191" s="20" t="s">
         <v>1</v>
@@ -15725,7 +15725,7 @@
         <v>1</v>
       </c>
       <c r="T192" s="16">
-        <v>170.87</v>
+        <v>15.87</v>
       </c>
       <c r="U192" s="20" t="s">
         <v>1</v>
@@ -15800,7 +15800,7 @@
         <v>1</v>
       </c>
       <c r="T193" s="16">
-        <v>171.87</v>
+        <v>15.87</v>
       </c>
       <c r="U193" s="20" t="s">
         <v>1</v>
@@ -15875,7 +15875,7 @@
         <v>1</v>
       </c>
       <c r="T194" s="16">
-        <v>172.87</v>
+        <v>15.87</v>
       </c>
       <c r="U194" s="20" t="s">
         <v>1</v>
@@ -15950,7 +15950,7 @@
         <v>1</v>
       </c>
       <c r="T195" s="16">
-        <v>173.87</v>
+        <v>15.87</v>
       </c>
       <c r="U195" s="20" t="s">
         <v>1</v>
@@ -16025,7 +16025,7 @@
         <v>1</v>
       </c>
       <c r="T196" s="16">
-        <v>174.87</v>
+        <v>15.87</v>
       </c>
       <c r="U196" s="20" t="s">
         <v>1</v>
@@ -16100,7 +16100,7 @@
         <v>1</v>
       </c>
       <c r="T197" s="16">
-        <v>175.87</v>
+        <v>15.87</v>
       </c>
       <c r="U197" s="20" t="s">
         <v>1</v>
@@ -16175,7 +16175,7 @@
         <v>1</v>
       </c>
       <c r="T198" s="16">
-        <v>176.87</v>
+        <v>15.87</v>
       </c>
       <c r="U198" s="20" t="s">
         <v>1</v>
@@ -16250,7 +16250,7 @@
         <v>1</v>
       </c>
       <c r="T199" s="16">
-        <v>177.87</v>
+        <v>15.87</v>
       </c>
       <c r="U199" s="20" t="s">
         <v>1</v>
@@ -16325,7 +16325,7 @@
         <v>1</v>
       </c>
       <c r="T200" s="16">
-        <v>178.87</v>
+        <v>15.87</v>
       </c>
       <c r="U200" s="20" t="s">
         <v>1</v>
@@ -16400,7 +16400,7 @@
         <v>1</v>
       </c>
       <c r="T201" s="16">
-        <v>179.87</v>
+        <v>15.87</v>
       </c>
       <c r="U201" s="20" t="s">
         <v>1</v>
@@ -16475,7 +16475,7 @@
         <v>1</v>
       </c>
       <c r="T202" s="16">
-        <v>180.87</v>
+        <v>15.87</v>
       </c>
       <c r="U202" s="20" t="s">
         <v>1</v>
@@ -16550,7 +16550,7 @@
         <v>1</v>
       </c>
       <c r="T203" s="16">
-        <v>181.87</v>
+        <v>15.87</v>
       </c>
       <c r="U203" s="20" t="s">
         <v>1</v>
@@ -16625,7 +16625,7 @@
         <v>1</v>
       </c>
       <c r="T204" s="16">
-        <v>182.87</v>
+        <v>15.87</v>
       </c>
       <c r="U204" s="20" t="s">
         <v>1</v>
@@ -16700,7 +16700,7 @@
         <v>1</v>
       </c>
       <c r="T205" s="16">
-        <v>183.87</v>
+        <v>15.87</v>
       </c>
       <c r="U205" s="20" t="s">
         <v>1</v>
@@ -16775,7 +16775,7 @@
         <v>1</v>
       </c>
       <c r="T206" s="16">
-        <v>184.87</v>
+        <v>15.87</v>
       </c>
       <c r="U206" s="20" t="s">
         <v>1</v>
@@ -16850,7 +16850,7 @@
         <v>1</v>
       </c>
       <c r="T207" s="16">
-        <v>185.87</v>
+        <v>15.87</v>
       </c>
       <c r="U207" s="20" t="s">
         <v>1</v>
@@ -16925,7 +16925,7 @@
         <v>1</v>
       </c>
       <c r="T208" s="16">
-        <v>186.87</v>
+        <v>15.87</v>
       </c>
       <c r="U208" s="20" t="s">
         <v>1</v>
@@ -17000,7 +17000,7 @@
         <v>1</v>
       </c>
       <c r="T209" s="16">
-        <v>187.87</v>
+        <v>15.87</v>
       </c>
       <c r="U209" s="20" t="s">
         <v>1</v>
@@ -17075,7 +17075,7 @@
         <v>1</v>
       </c>
       <c r="T210" s="16">
-        <v>188.87</v>
+        <v>15.87</v>
       </c>
       <c r="U210" s="20" t="s">
         <v>1</v>
@@ -17150,7 +17150,7 @@
         <v>1</v>
       </c>
       <c r="T211" s="16">
-        <v>189.87</v>
+        <v>15.87</v>
       </c>
       <c r="U211" s="20" t="s">
         <v>1</v>
@@ -17225,7 +17225,7 @@
         <v>1</v>
       </c>
       <c r="T212" s="16">
-        <v>190.87</v>
+        <v>15.87</v>
       </c>
       <c r="U212" s="20" t="s">
         <v>1</v>
@@ -17300,7 +17300,7 @@
         <v>1</v>
       </c>
       <c r="T213" s="16">
-        <v>191.87</v>
+        <v>15.87</v>
       </c>
       <c r="U213" s="20" t="s">
         <v>1</v>
@@ -17375,7 +17375,7 @@
         <v>1</v>
       </c>
       <c r="T214" s="16">
-        <v>192.87</v>
+        <v>15.87</v>
       </c>
       <c r="U214" s="20" t="s">
         <v>1</v>
@@ -17450,7 +17450,7 @@
         <v>1</v>
       </c>
       <c r="T215" s="16">
-        <v>193.87</v>
+        <v>15.87</v>
       </c>
       <c r="U215" s="20" t="s">
         <v>1</v>
@@ -17525,7 +17525,7 @@
         <v>1</v>
       </c>
       <c r="T216" s="16">
-        <v>194.87</v>
+        <v>15.87</v>
       </c>
       <c r="U216" s="20" t="s">
         <v>1</v>
@@ -17600,7 +17600,7 @@
         <v>1</v>
       </c>
       <c r="T217" s="16">
-        <v>195.87</v>
+        <v>15.87</v>
       </c>
       <c r="U217" s="20" t="s">
         <v>1</v>
@@ -26580,7 +26580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DA40484-3319-4556-998F-B01A9379511C}">
   <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>

</xml_diff>